<commit_message>
corrected error in data (AAL passenger revenue was incorrect for 2015-2017)
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4D3BB7F-0713-4601-95EF-B78465E448D8}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90CF029C-4E23-4F01-8DCB-F443B045FC35}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -631,6 +631,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -950,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4239,7 +4243,7 @@
         <v>42207000000</v>
       </c>
       <c r="E101">
-        <v>29238000000</v>
+        <v>36133000000</v>
       </c>
       <c r="F101">
         <v>38149000000</v>
@@ -4274,7 +4278,7 @@
         <v>40180000000</v>
       </c>
       <c r="E102">
-        <v>27909000000</v>
+        <v>34579000000</v>
       </c>
       <c r="F102">
         <v>34896000000</v>
@@ -4309,7 +4313,7 @@
         <v>40990000000</v>
       </c>
       <c r="E103">
-        <v>29037000000</v>
+        <v>35512000000</v>
       </c>
       <c r="F103">
         <v>34786000000</v>

</xml_diff>

<commit_message>
adds additional data (quarterly data for AAL, DAL, UAL back to 2014). provides additional explanation in the about section. adds estimations of quarterly profit sharing data based on annual reportings for quarters that AAL and UAL did not report.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/US Airlines Financials Project/airline_financials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90CF029C-4E23-4F01-8DCB-F443B045FC35}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5E31E5-FBE2-47E4-BE68-399B845649D8}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="18">
   <si>
     <t>Year</t>
   </si>
@@ -571,7 +571,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -952,27 +953,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
-  <dimension ref="A1:K125"/>
+  <dimension ref="A1:K173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2049,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2081,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2177,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2273,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2337,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2369,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2404,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2439,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2474,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2506,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2570,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2634,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2730,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2794,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2826,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2858,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2893,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2963,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3088,10 +3089,10 @@
         <v>66163000000</v>
       </c>
       <c r="K65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3184,10 +3185,10 @@
         <v>68567000000</v>
       </c>
       <c r="K68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>59000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3219,7 +3220,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3251,7 +3252,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3280,10 +3281,10 @@
         <v>65962000000</v>
       </c>
       <c r="K71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+        <v>88000000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3315,7 +3316,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3347,7 +3348,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3382,7 +3383,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3481,10 +3482,10 @@
         <v>65006000000</v>
       </c>
       <c r="K77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+        <v>35000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3577,10 +3578,10 @@
         <v>69658000000</v>
       </c>
       <c r="K80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+        <v>173000000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3644,7 +3645,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3676,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3708,7 +3709,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3740,7 +3741,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3769,10 +3770,10 @@
         <v>69773000000</v>
       </c>
       <c r="K86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+        <v>53000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3804,7 +3805,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3871,7 +3872,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3906,7 +3907,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4005,7 +4006,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4037,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4069,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4101,7 +4102,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4133,7 +4134,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4165,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4197,7 +4198,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4229,7 +4230,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4252,10 +4253,10 @@
         <v>1919000000</v>
       </c>
       <c r="H101">
-        <v>201351000000</v>
+        <v>226346000000</v>
       </c>
       <c r="I101">
-        <v>243806000000</v>
+        <v>276493000000</v>
       </c>
       <c r="J101">
         <v>22511000000</v>
@@ -4264,7 +4265,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4287,10 +4288,10 @@
         <v>2676000000</v>
       </c>
       <c r="H102">
-        <v>199014000000</v>
+        <v>223477000000</v>
       </c>
       <c r="I102">
-        <v>241734000000</v>
+        <v>273410000000</v>
       </c>
       <c r="J102">
         <v>22489000000</v>
@@ -4299,7 +4300,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4322,10 +4323,10 @@
         <v>7610000000</v>
       </c>
       <c r="H103">
-        <v>199467000000</v>
+        <v>223010000000</v>
       </c>
       <c r="I103">
-        <v>239375000000</v>
+        <v>268736000000</v>
       </c>
       <c r="J103">
         <v>18330000000</v>
@@ -4334,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4357,10 +4358,10 @@
         <v>2882000000</v>
       </c>
       <c r="H104">
-        <v>195651000000</v>
+        <v>217870000000</v>
       </c>
       <c r="I104">
-        <v>237522000000</v>
+        <v>265657000000</v>
       </c>
       <c r="J104">
         <v>16043000000</v>
@@ -4369,7 +4370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4404,7 +4405,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4439,7 +4440,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4474,7 +4475,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4509,7 +4510,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4532,10 +4533,10 @@
         <v>2131000000</v>
       </c>
       <c r="H109">
-        <v>193444000000</v>
+        <v>216261000000</v>
       </c>
       <c r="I109">
-        <v>234576000000</v>
+        <v>262386000000</v>
       </c>
       <c r="J109">
         <v>11703000000</v>
@@ -4544,7 +4545,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4567,10 +4568,10 @@
         <v>2263000000</v>
       </c>
       <c r="H110">
-        <v>186181000000</v>
+        <v>210309000000</v>
       </c>
       <c r="I110">
-        <v>224692000000</v>
+        <v>253590000000</v>
       </c>
       <c r="J110">
         <v>9918000000</v>
@@ -4579,7 +4580,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4602,10 +4603,10 @@
         <v>7340000000</v>
       </c>
       <c r="H111">
-        <v>183642000000</v>
+        <v>208611000000</v>
       </c>
       <c r="I111">
-        <v>219989000000</v>
+        <v>250003000000</v>
       </c>
       <c r="J111">
         <v>9673000000</v>
@@ -4614,7 +4615,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4637,10 +4638,10 @@
         <v>1132000000</v>
       </c>
       <c r="H112">
-        <v>179015000000</v>
+        <v>205559000000</v>
       </c>
       <c r="I112">
-        <v>214105000000</v>
+        <v>246021000000</v>
       </c>
       <c r="J112">
         <v>9953000000</v>
@@ -4649,7 +4650,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4684,7 +4685,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4719,7 +4720,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4754,7 +4755,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4789,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4824,7 +4825,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4859,7 +4860,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4894,7 +4895,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4929,7 +4930,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4964,7 +4965,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5031,7 +5032,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5093,6 +5094,1590 @@
       </c>
       <c r="K125">
         <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B126" s="1">
+        <v>1</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" s="1">
+        <v>9624000000</v>
+      </c>
+      <c r="E126" s="1">
+        <v>8155000000</v>
+      </c>
+      <c r="F126" s="1">
+        <v>9023000000</v>
+      </c>
+      <c r="G126" s="1">
+        <v>234000000</v>
+      </c>
+      <c r="H126" s="1">
+        <v>50984000000</v>
+      </c>
+      <c r="I126" s="1">
+        <v>64341000000</v>
+      </c>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1">
+        <v>31000000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" s="1">
+        <v>11105000000</v>
+      </c>
+      <c r="E127" s="1">
+        <v>9582000000</v>
+      </c>
+      <c r="F127" s="1">
+        <v>9570000000</v>
+      </c>
+      <c r="G127" s="1">
+        <v>803000000</v>
+      </c>
+      <c r="H127" s="1">
+        <v>59564000000</v>
+      </c>
+      <c r="I127" s="1">
+        <v>71743000000</v>
+      </c>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1">
+        <v>94000000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B128" s="1">
+        <v>3</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="1">
+        <v>10878000000</v>
+      </c>
+      <c r="E128" s="1">
+        <v>9377000000</v>
+      </c>
+      <c r="F128" s="1">
+        <v>9646000000</v>
+      </c>
+      <c r="G128" s="1">
+        <v>624000000</v>
+      </c>
+      <c r="H128" s="1">
+        <v>54012000000</v>
+      </c>
+      <c r="I128" s="1">
+        <v>64582000000</v>
+      </c>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1">
+        <v>70000000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B129" s="1">
+        <v>4</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" s="1">
+        <v>10600000000</v>
+      </c>
+      <c r="E129" s="1">
+        <v>9019000000</v>
+      </c>
+      <c r="F129" s="1">
+        <v>9910000000</v>
+      </c>
+      <c r="G129" s="1">
+        <v>258000000</v>
+      </c>
+      <c r="H129" s="1">
+        <v>55327000000</v>
+      </c>
+      <c r="I129" s="1">
+        <v>67355000000</v>
+      </c>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1">
+        <v>46700000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B130" s="1">
+        <v>1</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" s="1">
+        <v>9435000000</v>
+      </c>
+      <c r="E130" s="1">
+        <v>8087000000</v>
+      </c>
+      <c r="F130" s="1">
+        <v>8100000000</v>
+      </c>
+      <c r="G130" s="1">
+        <v>700000000</v>
+      </c>
+      <c r="H130" s="1">
+        <v>51771000000</v>
+      </c>
+      <c r="I130" s="1">
+        <v>65064000000</v>
+      </c>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1">
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B131" s="1">
+        <v>2</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131" s="1">
+        <v>10363000000</v>
+      </c>
+      <c r="E131" s="1">
+        <v>8995000000</v>
+      </c>
+      <c r="F131" s="1">
+        <v>8612000000</v>
+      </c>
+      <c r="G131" s="1">
+        <v>950000000</v>
+      </c>
+      <c r="H131" s="1">
+        <v>58336000000</v>
+      </c>
+      <c r="I131" s="1">
+        <v>70751000000</v>
+      </c>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1">
+        <v>98000000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B132" s="1">
+        <v>3</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D132" s="1">
+        <v>10594000000</v>
+      </c>
+      <c r="E132" s="1">
+        <v>9150000000</v>
+      </c>
+      <c r="F132" s="1">
+        <v>9163000000</v>
+      </c>
+      <c r="G132" s="1">
+        <v>737000000</v>
+      </c>
+      <c r="H132" s="1">
+        <v>53472000000</v>
+      </c>
+      <c r="I132" s="1">
+        <v>63751000000</v>
+      </c>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1">
+        <v>86000000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" s="1">
+        <v>9789000000</v>
+      </c>
+      <c r="E133" s="1">
+        <v>8347000000</v>
+      </c>
+      <c r="F133" s="1">
+        <v>9022000000</v>
+      </c>
+      <c r="G133" s="1">
+        <v>289000000</v>
+      </c>
+      <c r="H133" s="1">
+        <v>53452000000</v>
+      </c>
+      <c r="I133" s="1">
+        <v>65683000000</v>
+      </c>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1">
+        <v>57000000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B134" s="1">
+        <v>1</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" s="1">
+        <v>9827000000</v>
+      </c>
+      <c r="E134" s="1">
+        <v>8441000000</v>
+      </c>
+      <c r="F134" s="1">
+        <v>8611000000</v>
+      </c>
+      <c r="G134" s="1">
+        <v>932000000</v>
+      </c>
+      <c r="H134" s="1">
+        <v>50190000000</v>
+      </c>
+      <c r="I134" s="1">
+        <v>62791000000</v>
+      </c>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B135" s="1">
+        <v>2</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" s="1">
+        <v>10827000000</v>
+      </c>
+      <c r="E135" s="1">
+        <v>9414000000</v>
+      </c>
+      <c r="F135" s="1">
+        <v>8906000000</v>
+      </c>
+      <c r="G135" s="1">
+        <v>1704000000</v>
+      </c>
+      <c r="H135" s="1">
+        <v>57821000000</v>
+      </c>
+      <c r="I135" s="1">
+        <v>69401000000</v>
+      </c>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B136" s="1">
+        <v>3</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="1">
+        <v>10706000000</v>
+      </c>
+      <c r="E136" s="1">
+        <v>9353000000</v>
+      </c>
+      <c r="F136" s="1">
+        <v>8707000000</v>
+      </c>
+      <c r="G136" s="1">
+        <v>1693000000</v>
+      </c>
+      <c r="H136" s="1">
+        <v>60866000000</v>
+      </c>
+      <c r="I136" s="1">
+        <v>71092000000</v>
+      </c>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B137" s="1">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D137" s="1">
+        <v>9630000000</v>
+      </c>
+      <c r="E137" s="1">
+        <v>8305000000</v>
+      </c>
+      <c r="F137" s="1">
+        <v>8562000000</v>
+      </c>
+      <c r="G137" s="1">
+        <v>3281000000</v>
+      </c>
+      <c r="H137" s="1">
+        <v>54133000000</v>
+      </c>
+      <c r="I137" s="1">
+        <v>65453000000</v>
+      </c>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A138" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B138" s="1">
+        <v>1</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" s="1">
+        <v>9995000000</v>
+      </c>
+      <c r="E138" s="1">
+        <v>8665000000</v>
+      </c>
+      <c r="F138" s="1">
+        <v>9265000000</v>
+      </c>
+      <c r="G138" s="1">
+        <v>480000000</v>
+      </c>
+      <c r="H138" s="1">
+        <v>50886000000</v>
+      </c>
+      <c r="I138" s="1">
+        <v>63392000000</v>
+      </c>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A139" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B139" s="1">
+        <v>2</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" s="1">
+        <v>11355000000</v>
+      </c>
+      <c r="E139" s="1">
+        <v>9920000000</v>
+      </c>
+      <c r="F139" s="1">
+        <v>9956000000</v>
+      </c>
+      <c r="G139" s="1">
+        <v>864000000</v>
+      </c>
+      <c r="H139" s="1">
+        <v>57194000000</v>
+      </c>
+      <c r="I139" s="1">
+        <v>68090000000</v>
+      </c>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A140" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B140" s="1">
+        <v>3</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" s="1">
+        <v>11139000000</v>
+      </c>
+      <c r="E140" s="1">
+        <v>9758000000</v>
+      </c>
+      <c r="F140" s="1">
+        <v>9879000000</v>
+      </c>
+      <c r="G140" s="1">
+        <v>942000000</v>
+      </c>
+      <c r="H140" s="1">
+        <v>57650000000</v>
+      </c>
+      <c r="I140" s="1">
+        <v>69120000000</v>
+      </c>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A141" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B141" s="1">
+        <v>4</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="1">
+        <v>10160000000</v>
+      </c>
+      <c r="E141" s="1">
+        <v>8782000000</v>
+      </c>
+      <c r="F141" s="1">
+        <v>9300000000</v>
+      </c>
+      <c r="G141" s="1">
+        <v>597000000</v>
+      </c>
+      <c r="H141" s="1">
+        <v>52140000000</v>
+      </c>
+      <c r="I141" s="1">
+        <v>65053000000</v>
+      </c>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A142" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B142" s="1">
+        <v>1</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" s="1">
+        <v>9148000000</v>
+      </c>
+      <c r="E142" s="1">
+        <v>7688000000</v>
+      </c>
+      <c r="F142" s="1">
+        <v>8095000000</v>
+      </c>
+      <c r="G142" s="1">
+        <v>603000000</v>
+      </c>
+      <c r="H142" s="1">
+        <v>47952000000</v>
+      </c>
+      <c r="I142" s="1">
+        <v>57871000000</v>
+      </c>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1">
+        <v>151000000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A143" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B143" s="1">
+        <v>2</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="1">
+        <v>10791000000</v>
+      </c>
+      <c r="E143" s="1">
+        <v>9231000000</v>
+      </c>
+      <c r="F143" s="1">
+        <v>8763000000</v>
+      </c>
+      <c r="G143" s="1">
+        <v>1224000000</v>
+      </c>
+      <c r="H143" s="1">
+        <v>57575000000</v>
+      </c>
+      <c r="I143" s="1">
+        <v>66227000000</v>
+      </c>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1">
+        <v>338000000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A144" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B144" s="1">
+        <v>3</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" s="1">
+        <v>11060000000</v>
+      </c>
+      <c r="E144" s="1">
+        <v>9399000000</v>
+      </c>
+      <c r="F144" s="1">
+        <v>9221000000</v>
+      </c>
+      <c r="G144" s="1">
+        <v>1178000000</v>
+      </c>
+      <c r="H144" s="1">
+        <v>61006000000</v>
+      </c>
+      <c r="I144" s="1">
+        <v>70167000000</v>
+      </c>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1">
+        <v>314000000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A145" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B145" s="1">
+        <v>4</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="1">
+        <v>10245000000</v>
+      </c>
+      <c r="E145" s="1">
+        <v>8501000000</v>
+      </c>
+      <c r="F145" s="1">
+        <v>9052000000</v>
+      </c>
+      <c r="G145" s="1">
+        <v>572000000</v>
+      </c>
+      <c r="H145" s="1">
+        <v>51180000000</v>
+      </c>
+      <c r="I145" s="1">
+        <v>60060000000</v>
+      </c>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1">
+        <v>262000000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A146" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B146" s="1">
+        <v>1</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="1">
+        <v>9251000000</v>
+      </c>
+      <c r="E146" s="1">
+        <v>7762000000</v>
+      </c>
+      <c r="F146" s="1">
+        <v>7711000000</v>
+      </c>
+      <c r="G146" s="1">
+        <v>946000000</v>
+      </c>
+      <c r="H146" s="1">
+        <v>47725000000</v>
+      </c>
+      <c r="I146" s="1">
+        <v>58145000000</v>
+      </c>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1">
+        <v>272000000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A147" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B147" s="1">
+        <v>2</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" s="1">
+        <v>10447000000</v>
+      </c>
+      <c r="E147" s="1">
+        <v>8970000000</v>
+      </c>
+      <c r="F147" s="1">
+        <v>8024000000</v>
+      </c>
+      <c r="G147" s="1">
+        <v>1546000000</v>
+      </c>
+      <c r="H147" s="1">
+        <v>56415000000</v>
+      </c>
+      <c r="I147" s="1">
+        <v>65979000000</v>
+      </c>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1">
+        <v>324000000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A148" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B148" s="1">
+        <v>3</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D148" s="1">
+        <v>10483000000</v>
+      </c>
+      <c r="E148" s="1">
+        <v>9071000000</v>
+      </c>
+      <c r="F148" s="1">
+        <v>8514000000</v>
+      </c>
+      <c r="G148" s="1">
+        <v>1259000000</v>
+      </c>
+      <c r="H148" s="1">
+        <v>58973000000</v>
+      </c>
+      <c r="I148" s="1">
+        <v>69028000000</v>
+      </c>
+      <c r="J148" s="1"/>
+      <c r="K148" s="1">
+        <v>326000000</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A149" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B149" s="1">
+        <v>4</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" s="1">
+        <v>9458000000</v>
+      </c>
+      <c r="E149" s="1">
+        <v>7974000000</v>
+      </c>
+      <c r="F149" s="1">
+        <v>8438000000</v>
+      </c>
+      <c r="G149" s="1">
+        <v>622000000</v>
+      </c>
+      <c r="H149" s="1">
+        <v>49985000000</v>
+      </c>
+      <c r="I149" s="1">
+        <v>58715000000</v>
+      </c>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1">
+        <v>193000000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A150" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B150" s="1">
+        <v>1</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="1">
+        <v>9388000000</v>
+      </c>
+      <c r="E150" s="1">
+        <v>7923000000</v>
+      </c>
+      <c r="F150" s="1">
+        <v>7990000000</v>
+      </c>
+      <c r="G150" s="1">
+        <v>746000000</v>
+      </c>
+      <c r="H150" s="1">
+        <v>46221000000</v>
+      </c>
+      <c r="I150" s="1">
+        <v>56597000000</v>
+      </c>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1">
+        <v>136000000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A151" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B151" s="1">
+        <v>2</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" s="1">
+        <v>10707000000</v>
+      </c>
+      <c r="E151" s="1">
+        <v>9139000000</v>
+      </c>
+      <c r="F151" s="1">
+        <v>8233000000</v>
+      </c>
+      <c r="G151" s="1">
+        <v>1485000000</v>
+      </c>
+      <c r="H151" s="1">
+        <v>54755000000</v>
+      </c>
+      <c r="I151" s="1">
+        <v>63937000000</v>
+      </c>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1">
+        <v>411000000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A152" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B152" s="1">
+        <v>3</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="1">
+        <v>11107000000</v>
+      </c>
+      <c r="E152" s="1">
+        <v>9595000000</v>
+      </c>
+      <c r="F152" s="1">
+        <v>8894000000</v>
+      </c>
+      <c r="G152" s="1">
+        <v>1315000000</v>
+      </c>
+      <c r="H152" s="1">
+        <v>59076000000</v>
+      </c>
+      <c r="I152" s="1">
+        <v>68031000000</v>
+      </c>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1">
+        <v>563000000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B153" s="1">
+        <v>4</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" s="1">
+        <v>9502000000</v>
+      </c>
+      <c r="E153" s="1">
+        <v>8125000000</v>
+      </c>
+      <c r="F153" s="1">
+        <v>7785000000</v>
+      </c>
+      <c r="G153" s="1">
+        <v>980000000</v>
+      </c>
+      <c r="H153" s="1">
+        <v>49573000000</v>
+      </c>
+      <c r="I153" s="1">
+        <v>58199000000</v>
+      </c>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1">
+        <v>380000000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B154" s="1">
+        <v>1</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" s="1">
+        <v>8916000000</v>
+      </c>
+      <c r="E154" s="1">
+        <v>7677000000</v>
+      </c>
+      <c r="F154" s="1">
+        <v>8296000000</v>
+      </c>
+      <c r="G154" s="1">
+        <v>213000000</v>
+      </c>
+      <c r="H154" s="1">
+        <v>44601000000</v>
+      </c>
+      <c r="I154" s="1">
+        <v>53904000000</v>
+      </c>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1">
+        <v>99000000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B155" s="1">
+        <v>2</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" s="1">
+        <v>10621000000</v>
+      </c>
+      <c r="E155" s="1">
+        <v>9266000000</v>
+      </c>
+      <c r="F155" s="1">
+        <v>9042000000</v>
+      </c>
+      <c r="G155" s="1">
+        <v>801000000</v>
+      </c>
+      <c r="H155" s="1">
+        <v>53341000000</v>
+      </c>
+      <c r="I155" s="1">
+        <v>61817000000</v>
+      </c>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1">
+        <v>340000000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B156" s="1">
+        <v>3</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D156" s="1">
+        <v>11178000000</v>
+      </c>
+      <c r="E156" s="1">
+        <v>9776000000</v>
+      </c>
+      <c r="F156" s="1">
+        <v>10343000000</v>
+      </c>
+      <c r="G156" s="1">
+        <v>357000000</v>
+      </c>
+      <c r="H156" s="1">
+        <v>56955000000</v>
+      </c>
+      <c r="I156" s="1">
+        <v>65926000000</v>
+      </c>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1">
+        <v>384000000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B157" s="1">
+        <v>4</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="1">
+        <v>9647000000</v>
+      </c>
+      <c r="E157" s="1">
+        <v>8235000000</v>
+      </c>
+      <c r="F157" s="1">
+        <v>10475000000</v>
+      </c>
+      <c r="G157" s="1">
+        <v>-712000000</v>
+      </c>
+      <c r="H157" s="1">
+        <v>48028000000</v>
+      </c>
+      <c r="I157" s="1">
+        <v>58029000000</v>
+      </c>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1">
+        <v>262000000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A158" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B158" s="1">
+        <v>1</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D158" s="1">
+        <v>8420000000</v>
+      </c>
+      <c r="E158" s="1">
+        <v>7174000000</v>
+      </c>
+      <c r="F158" s="1">
+        <v>8142000000</v>
+      </c>
+      <c r="G158" s="1">
+        <v>96000000</v>
+      </c>
+      <c r="H158" s="1">
+        <v>47611000000</v>
+      </c>
+      <c r="I158" s="1">
+        <v>59808000000</v>
+      </c>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1">
+        <v>28000000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A159" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B159" s="1">
+        <v>2</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D159" s="1">
+        <v>10000000000</v>
+      </c>
+      <c r="E159" s="1">
+        <v>8622000000</v>
+      </c>
+      <c r="F159" s="1">
+        <v>8601000000</v>
+      </c>
+      <c r="G159" s="1">
+        <v>818000000</v>
+      </c>
+      <c r="H159" s="1">
+        <v>56356000000</v>
+      </c>
+      <c r="I159" s="1">
+        <v>67467000000</v>
+      </c>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1">
+        <v>140000000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A160" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B160" s="1">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D160" s="1">
+        <v>9878000000</v>
+      </c>
+      <c r="E160" s="1">
+        <v>8528000000</v>
+      </c>
+      <c r="F160" s="1">
+        <v>8786000000</v>
+      </c>
+      <c r="G160" s="1">
+        <v>637000000</v>
+      </c>
+      <c r="H160" s="1">
+        <v>59145000000</v>
+      </c>
+      <c r="I160" s="1">
+        <v>70083000000</v>
+      </c>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1">
+        <v>109000000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A161" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B161" s="1">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D161" s="1">
+        <v>9438000000</v>
+      </c>
+      <c r="E161" s="1">
+        <v>8080000000</v>
+      </c>
+      <c r="F161" s="1">
+        <v>8709000000</v>
+      </c>
+      <c r="G161" s="1">
+        <v>580000000</v>
+      </c>
+      <c r="H161" s="1">
+        <v>53149000000</v>
+      </c>
+      <c r="I161" s="1">
+        <v>65028000000</v>
+      </c>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1">
+        <v>73000000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A162" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B162" s="1">
+        <v>1</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D162" s="1">
+        <v>8195000000</v>
+      </c>
+      <c r="E162" s="1">
+        <v>6990000000</v>
+      </c>
+      <c r="F162" s="1">
+        <v>7546000000</v>
+      </c>
+      <c r="G162" s="1">
+        <v>313000000</v>
+      </c>
+      <c r="H162" s="1">
+        <v>46582000000</v>
+      </c>
+      <c r="I162" s="1">
+        <v>58273000000</v>
+      </c>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1">
+        <v>94000000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A163" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B163" s="1">
+        <v>2</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" s="1">
+        <v>9396000000</v>
+      </c>
+      <c r="E163" s="1">
+        <v>8103000000</v>
+      </c>
+      <c r="F163" s="1">
+        <v>8336000000</v>
+      </c>
+      <c r="G163" s="1">
+        <v>588000000</v>
+      </c>
+      <c r="H163" s="1">
+        <v>54017000000</v>
+      </c>
+      <c r="I163" s="1">
+        <v>64725000000</v>
+      </c>
+      <c r="J163" s="1"/>
+      <c r="K163" s="1">
+        <v>153000000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A164" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B164" s="1">
+        <v>3</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" s="1">
+        <v>9913000000</v>
+      </c>
+      <c r="E164" s="1">
+        <v>8603000000</v>
+      </c>
+      <c r="F164" s="1">
+        <v>8289000000</v>
+      </c>
+      <c r="G164" s="1">
+        <v>965000000</v>
+      </c>
+      <c r="H164" s="1">
+        <v>58172000000</v>
+      </c>
+      <c r="I164" s="1">
+        <v>68074000000</v>
+      </c>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1">
+        <v>235000000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A165" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B165" s="1">
+        <v>4</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D165" s="1">
+        <v>9052000000</v>
+      </c>
+      <c r="E165" s="1">
+        <v>7761000000</v>
+      </c>
+      <c r="F165" s="1">
+        <v>8047000000</v>
+      </c>
+      <c r="G165" s="1">
+        <v>397000000</v>
+      </c>
+      <c r="H165" s="1">
+        <v>51538000000</v>
+      </c>
+      <c r="I165" s="1">
+        <v>62518000000</v>
+      </c>
+      <c r="J165" s="1"/>
+      <c r="K165" s="1">
+        <v>145000000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A166" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B166" s="1">
+        <v>1</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" s="1">
+        <v>8608000000</v>
+      </c>
+      <c r="E166" s="1">
+        <v>7420000000</v>
+      </c>
+      <c r="F166" s="1">
+        <v>7867000000</v>
+      </c>
+      <c r="G166" s="1">
+        <v>508000000</v>
+      </c>
+      <c r="H166" s="1">
+        <v>46444000000</v>
+      </c>
+      <c r="I166" s="1">
+        <v>57269000000</v>
+      </c>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A167" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B167" s="1">
+        <v>2</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D167" s="1">
+        <v>9914000000</v>
+      </c>
+      <c r="E167" s="1">
+        <v>8676000000</v>
+      </c>
+      <c r="F167" s="1">
+        <v>8469000000</v>
+      </c>
+      <c r="G167" s="1">
+        <v>1193000000</v>
+      </c>
+      <c r="H167" s="1">
+        <v>54289000000</v>
+      </c>
+      <c r="I167" s="1">
+        <v>64685000000</v>
+      </c>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1">
+        <v>195000000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A168" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B168" s="1">
+        <v>3</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D168" s="1">
+        <v>10306000000</v>
+      </c>
+      <c r="E168" s="1">
+        <v>8960000000</v>
+      </c>
+      <c r="F168" s="1">
+        <v>8407000000</v>
+      </c>
+      <c r="G168" s="1">
+        <v>4816000000</v>
+      </c>
+      <c r="H168" s="1">
+        <v>57160000000</v>
+      </c>
+      <c r="I168" s="1">
+        <v>66745000000</v>
+      </c>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1">
+        <v>257000000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A169" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B169" s="1">
+        <v>4</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D169" s="1">
+        <v>9036000000</v>
+      </c>
+      <c r="E169" s="1">
+        <v>7729000000</v>
+      </c>
+      <c r="F169" s="1">
+        <v>7955000000</v>
+      </c>
+      <c r="G169" s="1">
+        <v>823000000</v>
+      </c>
+      <c r="H169" s="1">
+        <v>50718000000</v>
+      </c>
+      <c r="I169" s="1">
+        <v>61304000000</v>
+      </c>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1">
+        <v>146000000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A170" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B170" s="1">
+        <v>1</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D170" s="1">
+        <v>8696000000</v>
+      </c>
+      <c r="E170" s="1">
+        <v>7384000000</v>
+      </c>
+      <c r="F170" s="1">
+        <v>9045000000</v>
+      </c>
+      <c r="G170" s="1">
+        <v>-609000000</v>
+      </c>
+      <c r="H170" s="1">
+        <v>46383000000</v>
+      </c>
+      <c r="I170" s="1">
+        <v>57216000000</v>
+      </c>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A171" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B171" s="1">
+        <v>2</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="1">
+        <v>10329000000</v>
+      </c>
+      <c r="E171" s="1">
+        <v>8981000000</v>
+      </c>
+      <c r="F171" s="1">
+        <v>9423000000</v>
+      </c>
+      <c r="G171" s="1">
+        <v>789000000</v>
+      </c>
+      <c r="H171" s="1">
+        <v>53900000000</v>
+      </c>
+      <c r="I171" s="1">
+        <v>63214000000</v>
+      </c>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1">
+        <v>78000000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A172" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B172" s="1">
+        <v>3</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D172" s="1">
+        <v>10563000000</v>
+      </c>
+      <c r="E172" s="1">
+        <v>9314000000</v>
+      </c>
+      <c r="F172" s="1">
+        <v>9372000000</v>
+      </c>
+      <c r="G172" s="1">
+        <v>924000000</v>
+      </c>
+      <c r="H172" s="1">
+        <v>56065000000</v>
+      </c>
+      <c r="I172" s="1">
+        <v>65378000000</v>
+      </c>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1">
+        <v>103000000</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A173" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B173" s="1">
+        <v>4</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D173" s="1">
+        <v>9313000000</v>
+      </c>
+      <c r="E173" s="1">
+        <v>8083000000</v>
+      </c>
+      <c r="F173" s="1">
+        <v>8688000000</v>
+      </c>
+      <c r="G173" s="1">
+        <v>28000000</v>
+      </c>
+      <c r="H173" s="1">
+        <v>49211000000</v>
+      </c>
+      <c r="I173" s="1">
+        <v>60213000000</v>
+      </c>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1">
+        <v>54000000</v>
       </c>
     </row>
   </sheetData>
@@ -5108,13 +6693,13 @@
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5131,7 +6716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -5148,7 +6733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -5165,7 +6750,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -5182,7 +6767,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -5199,7 +6784,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -5216,7 +6801,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -5233,7 +6818,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -5250,7 +6835,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -5267,7 +6852,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -5284,7 +6869,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -5301,7 +6886,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -5318,7 +6903,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -5335,7 +6920,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -5352,7 +6937,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -5369,7 +6954,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -5386,7 +6971,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -5403,7 +6988,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -5420,7 +7005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -5437,7 +7022,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -5454,7 +7039,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -5471,7 +7056,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -5488,7 +7073,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -5505,7 +7090,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -5522,7 +7107,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>

</xml_diff>

<commit_message>
adjusts how metric definitions are displayed
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5E31E5-FBE2-47E4-BE68-399B845649D8}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49AE8822-1526-4537-8620-2DD0DDB42906}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -571,8 +571,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -955,25 +954,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K87" sqref="K87"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O125" sqref="O125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1040,7 +1038,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1104,7 +1102,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1136,7 +1134,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1168,7 +1166,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1200,7 +1198,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1264,7 +1262,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1296,7 +1294,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1328,7 +1326,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1360,7 +1358,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1392,7 +1390,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1427,7 +1425,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1462,7 +1460,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1497,7 +1495,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1529,7 +1527,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1561,7 +1559,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1593,7 +1591,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1625,7 +1623,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1657,7 +1655,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1689,7 +1687,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1721,7 +1719,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1753,7 +1751,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1785,7 +1783,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1817,7 +1815,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1849,7 +1847,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1881,7 +1879,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1916,7 +1914,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1951,7 +1949,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1986,7 +1984,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2018,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2050,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2082,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2114,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2146,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2178,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2210,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2242,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2274,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2306,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2338,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2370,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2405,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2440,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2475,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2507,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2539,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2571,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2603,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2635,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2667,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2699,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2731,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2763,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2795,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2827,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2859,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2894,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2929,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2964,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -2996,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3028,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3060,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3092,7 +3090,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3124,7 +3122,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3156,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3188,7 +3186,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3220,7 +3218,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3252,7 +3250,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3284,7 +3282,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3316,7 +3314,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3348,7 +3346,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3383,7 +3381,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3418,7 +3416,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3453,7 +3451,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3485,7 +3483,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3517,7 +3515,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3549,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3581,7 +3579,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3613,7 +3611,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3645,7 +3643,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3677,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3709,7 +3707,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3741,7 +3739,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3773,7 +3771,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3805,7 +3803,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3837,7 +3835,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3872,7 +3870,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3907,7 +3905,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3942,7 +3940,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3974,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4006,7 +4004,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4038,7 +4036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4070,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4102,7 +4100,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4134,7 +4132,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4166,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4198,7 +4196,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4230,7 +4228,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4265,7 +4263,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4300,7 +4298,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4335,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4370,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4405,7 +4403,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4440,7 +4438,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4475,7 +4473,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4510,7 +4508,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4545,7 +4543,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4580,7 +4578,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4615,7 +4613,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4650,7 +4648,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4720,7 +4718,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4755,7 +4753,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4790,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4825,7 +4823,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4860,7 +4858,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4895,7 +4893,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4930,7 +4928,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4965,7 +4963,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5000,7 +4998,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5032,7 +5030,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5064,7 +5062,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5096,1587 +5094,1539 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126" s="1">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126">
         <v>2017</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126">
         <v>1</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" t="s">
         <v>6</v>
       </c>
-      <c r="D126" s="1">
+      <c r="D126">
         <v>9624000000</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126">
         <v>8155000000</v>
       </c>
-      <c r="F126" s="1">
+      <c r="F126">
         <v>9023000000</v>
       </c>
-      <c r="G126" s="1">
+      <c r="G126">
         <v>234000000</v>
       </c>
-      <c r="H126" s="1">
+      <c r="H126">
         <v>50984000000</v>
       </c>
-      <c r="I126" s="1">
+      <c r="I126">
         <v>64341000000</v>
       </c>
-      <c r="J126" s="1"/>
-      <c r="K126" s="1">
+      <c r="K126">
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A127" s="1">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127">
         <v>2017</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127">
         <v>2</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" t="s">
         <v>6</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D127">
         <v>11105000000</v>
       </c>
-      <c r="E127" s="1">
+      <c r="E127">
         <v>9582000000</v>
       </c>
-      <c r="F127" s="1">
+      <c r="F127">
         <v>9570000000</v>
       </c>
-      <c r="G127" s="1">
+      <c r="G127">
         <v>803000000</v>
       </c>
-      <c r="H127" s="1">
+      <c r="H127">
         <v>59564000000</v>
       </c>
-      <c r="I127" s="1">
+      <c r="I127">
         <v>71743000000</v>
       </c>
-      <c r="J127" s="1"/>
-      <c r="K127" s="1">
+      <c r="K127">
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A128" s="1">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128">
         <v>2017</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128">
         <v>3</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" t="s">
         <v>6</v>
       </c>
-      <c r="D128" s="1">
+      <c r="D128">
         <v>10878000000</v>
       </c>
-      <c r="E128" s="1">
+      <c r="E128">
         <v>9377000000</v>
       </c>
-      <c r="F128" s="1">
+      <c r="F128">
         <v>9646000000</v>
       </c>
-      <c r="G128" s="1">
+      <c r="G128">
         <v>624000000</v>
       </c>
-      <c r="H128" s="1">
+      <c r="H128">
         <v>54012000000</v>
       </c>
-      <c r="I128" s="1">
+      <c r="I128">
         <v>64582000000</v>
       </c>
-      <c r="J128" s="1"/>
-      <c r="K128" s="1">
+      <c r="K128">
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A129" s="1">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129">
         <v>2017</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129">
         <v>4</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" t="s">
         <v>6</v>
       </c>
-      <c r="D129" s="1">
+      <c r="D129">
         <v>10600000000</v>
       </c>
-      <c r="E129" s="1">
+      <c r="E129">
         <v>9019000000</v>
       </c>
-      <c r="F129" s="1">
+      <c r="F129">
         <v>9910000000</v>
       </c>
-      <c r="G129" s="1">
+      <c r="G129">
         <v>258000000</v>
       </c>
-      <c r="H129" s="1">
+      <c r="H129">
         <v>55327000000</v>
       </c>
-      <c r="I129" s="1">
+      <c r="I129">
         <v>67355000000</v>
       </c>
-      <c r="J129" s="1"/>
-      <c r="K129" s="1">
-        <v>46700000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A130" s="1">
+      <c r="K129">
+        <v>47000000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130">
         <v>2016</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130">
         <v>1</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" t="s">
         <v>6</v>
       </c>
-      <c r="D130" s="1">
+      <c r="D130">
         <v>9435000000</v>
       </c>
-      <c r="E130" s="1">
+      <c r="E130">
         <v>8087000000</v>
       </c>
-      <c r="F130" s="1">
+      <c r="F130">
         <v>8100000000</v>
       </c>
-      <c r="G130" s="1">
+      <c r="G130">
         <v>700000000</v>
       </c>
-      <c r="H130" s="1">
+      <c r="H130">
         <v>51771000000</v>
       </c>
-      <c r="I130" s="1">
+      <c r="I130">
         <v>65064000000</v>
       </c>
-      <c r="J130" s="1"/>
-      <c r="K130" s="1">
+      <c r="K130">
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A131" s="1">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131">
         <v>2016</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131">
         <v>2</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" t="s">
         <v>6</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D131">
         <v>10363000000</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131">
         <v>8995000000</v>
       </c>
-      <c r="F131" s="1">
+      <c r="F131">
         <v>8612000000</v>
       </c>
-      <c r="G131" s="1">
+      <c r="G131">
         <v>950000000</v>
       </c>
-      <c r="H131" s="1">
+      <c r="H131">
         <v>58336000000</v>
       </c>
-      <c r="I131" s="1">
+      <c r="I131">
         <v>70751000000</v>
       </c>
-      <c r="J131" s="1"/>
-      <c r="K131" s="1">
+      <c r="K131">
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A132" s="1">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132">
         <v>2016</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132">
         <v>3</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" t="s">
         <v>6</v>
       </c>
-      <c r="D132" s="1">
+      <c r="D132">
         <v>10594000000</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132">
         <v>9150000000</v>
       </c>
-      <c r="F132" s="1">
+      <c r="F132">
         <v>9163000000</v>
       </c>
-      <c r="G132" s="1">
+      <c r="G132">
         <v>737000000</v>
       </c>
-      <c r="H132" s="1">
+      <c r="H132">
         <v>53472000000</v>
       </c>
-      <c r="I132" s="1">
+      <c r="I132">
         <v>63751000000</v>
       </c>
-      <c r="J132" s="1"/>
-      <c r="K132" s="1">
+      <c r="K132">
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A133" s="1">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A133">
         <v>2016</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B133">
         <v>4</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" t="s">
         <v>6</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133">
         <v>9789000000</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133">
         <v>8347000000</v>
       </c>
-      <c r="F133" s="1">
+      <c r="F133">
         <v>9022000000</v>
       </c>
-      <c r="G133" s="1">
+      <c r="G133">
         <v>289000000</v>
       </c>
-      <c r="H133" s="1">
+      <c r="H133">
         <v>53452000000</v>
       </c>
-      <c r="I133" s="1">
+      <c r="I133">
         <v>65683000000</v>
       </c>
-      <c r="J133" s="1"/>
-      <c r="K133" s="1">
+      <c r="K133">
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A134" s="1">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134">
         <v>2015</v>
       </c>
-      <c r="B134" s="1">
+      <c r="B134">
         <v>1</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" t="s">
         <v>6</v>
       </c>
-      <c r="D134" s="1">
+      <c r="D134">
         <v>9827000000</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134">
         <v>8441000000</v>
       </c>
-      <c r="F134" s="1">
+      <c r="F134">
         <v>8611000000</v>
       </c>
-      <c r="G134" s="1">
+      <c r="G134">
         <v>932000000</v>
       </c>
-      <c r="H134" s="1">
+      <c r="H134">
         <v>50190000000</v>
       </c>
-      <c r="I134" s="1">
+      <c r="I134">
         <v>62791000000</v>
       </c>
-      <c r="J134" s="1"/>
-      <c r="K134" s="1">
+      <c r="K134">
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A135" s="1">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135">
         <v>2015</v>
       </c>
-      <c r="B135" s="1">
+      <c r="B135">
         <v>2</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" t="s">
         <v>6</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135">
         <v>10827000000</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135">
         <v>9414000000</v>
       </c>
-      <c r="F135" s="1">
+      <c r="F135">
         <v>8906000000</v>
       </c>
-      <c r="G135" s="1">
+      <c r="G135">
         <v>1704000000</v>
       </c>
-      <c r="H135" s="1">
+      <c r="H135">
         <v>57821000000</v>
       </c>
-      <c r="I135" s="1">
+      <c r="I135">
         <v>69401000000</v>
       </c>
-      <c r="J135" s="1"/>
-      <c r="K135" s="1">
+      <c r="K135">
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A136" s="1">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136">
         <v>2015</v>
       </c>
-      <c r="B136" s="1">
+      <c r="B136">
         <v>3</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" t="s">
         <v>6</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D136">
         <v>10706000000</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136">
         <v>9353000000</v>
       </c>
-      <c r="F136" s="1">
+      <c r="F136">
         <v>8707000000</v>
       </c>
-      <c r="G136" s="1">
+      <c r="G136">
         <v>1693000000</v>
       </c>
-      <c r="H136" s="1">
+      <c r="H136">
         <v>60866000000</v>
       </c>
-      <c r="I136" s="1">
+      <c r="I136">
         <v>71092000000</v>
       </c>
-      <c r="J136" s="1"/>
-      <c r="K136" s="1">
+      <c r="K136">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A137" s="1">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137">
         <v>2015</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137">
         <v>4</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" t="s">
         <v>6</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137">
         <v>9630000000</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137">
         <v>8305000000</v>
       </c>
-      <c r="F137" s="1">
+      <c r="F137">
         <v>8562000000</v>
       </c>
-      <c r="G137" s="1">
+      <c r="G137">
         <v>3281000000</v>
       </c>
-      <c r="H137" s="1">
+      <c r="H137">
         <v>54133000000</v>
       </c>
-      <c r="I137" s="1">
+      <c r="I137">
         <v>65453000000</v>
       </c>
-      <c r="J137" s="1"/>
-      <c r="K137" s="1">
+      <c r="K137">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A138" s="1">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138">
         <v>2014</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138">
         <v>1</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" t="s">
         <v>6</v>
       </c>
-      <c r="D138" s="1">
+      <c r="D138">
         <v>9995000000</v>
       </c>
-      <c r="E138" s="1">
+      <c r="E138">
         <v>8665000000</v>
       </c>
-      <c r="F138" s="1">
+      <c r="F138">
         <v>9265000000</v>
       </c>
-      <c r="G138" s="1">
+      <c r="G138">
         <v>480000000</v>
       </c>
-      <c r="H138" s="1">
+      <c r="H138">
         <v>50886000000</v>
       </c>
-      <c r="I138" s="1">
+      <c r="I138">
         <v>63392000000</v>
       </c>
-      <c r="J138" s="1"/>
-      <c r="K138" s="1">
+      <c r="K138">
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A139" s="1">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139">
         <v>2014</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139">
         <v>2</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" t="s">
         <v>6</v>
       </c>
-      <c r="D139" s="1">
+      <c r="D139">
         <v>11355000000</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139">
         <v>9920000000</v>
       </c>
-      <c r="F139" s="1">
+      <c r="F139">
         <v>9956000000</v>
       </c>
-      <c r="G139" s="1">
+      <c r="G139">
         <v>864000000</v>
       </c>
-      <c r="H139" s="1">
+      <c r="H139">
         <v>57194000000</v>
       </c>
-      <c r="I139" s="1">
+      <c r="I139">
         <v>68090000000</v>
       </c>
-      <c r="J139" s="1"/>
-      <c r="K139" s="1">
+      <c r="K139">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A140" s="1">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140">
         <v>2014</v>
       </c>
-      <c r="B140" s="1">
+      <c r="B140">
         <v>3</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C140" t="s">
         <v>6</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D140">
         <v>11139000000</v>
       </c>
-      <c r="E140" s="1">
+      <c r="E140">
         <v>9758000000</v>
       </c>
-      <c r="F140" s="1">
+      <c r="F140">
         <v>9879000000</v>
       </c>
-      <c r="G140" s="1">
+      <c r="G140">
         <v>942000000</v>
       </c>
-      <c r="H140" s="1">
+      <c r="H140">
         <v>57650000000</v>
       </c>
-      <c r="I140" s="1">
+      <c r="I140">
         <v>69120000000</v>
       </c>
-      <c r="J140" s="1"/>
-      <c r="K140" s="1">
+      <c r="K140">
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A141" s="1">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141">
         <v>2014</v>
       </c>
-      <c r="B141" s="1">
+      <c r="B141">
         <v>4</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" t="s">
         <v>6</v>
       </c>
-      <c r="D141" s="1">
+      <c r="D141">
         <v>10160000000</v>
       </c>
-      <c r="E141" s="1">
+      <c r="E141">
         <v>8782000000</v>
       </c>
-      <c r="F141" s="1">
+      <c r="F141">
         <v>9300000000</v>
       </c>
-      <c r="G141" s="1">
+      <c r="G141">
         <v>597000000</v>
       </c>
-      <c r="H141" s="1">
+      <c r="H141">
         <v>52140000000</v>
       </c>
-      <c r="I141" s="1">
+      <c r="I141">
         <v>65053000000</v>
       </c>
-      <c r="J141" s="1"/>
-      <c r="K141" s="1">
+      <c r="K141">
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A142" s="1">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142">
         <v>2017</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B142">
         <v>1</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" t="s">
         <v>7</v>
       </c>
-      <c r="D142" s="1">
+      <c r="D142">
         <v>9148000000</v>
       </c>
-      <c r="E142" s="1">
+      <c r="E142">
         <v>7688000000</v>
       </c>
-      <c r="F142" s="1">
+      <c r="F142">
         <v>8095000000</v>
       </c>
-      <c r="G142" s="1">
+      <c r="G142">
         <v>603000000</v>
       </c>
-      <c r="H142" s="1">
+      <c r="H142">
         <v>47952000000</v>
       </c>
-      <c r="I142" s="1">
+      <c r="I142">
         <v>57871000000</v>
       </c>
-      <c r="J142" s="1"/>
-      <c r="K142" s="1">
+      <c r="K142">
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A143" s="1">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143">
         <v>2017</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143">
         <v>2</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" t="s">
         <v>7</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D143">
         <v>10791000000</v>
       </c>
-      <c r="E143" s="1">
+      <c r="E143">
         <v>9231000000</v>
       </c>
-      <c r="F143" s="1">
+      <c r="F143">
         <v>8763000000</v>
       </c>
-      <c r="G143" s="1">
+      <c r="G143">
         <v>1224000000</v>
       </c>
-      <c r="H143" s="1">
+      <c r="H143">
         <v>57575000000</v>
       </c>
-      <c r="I143" s="1">
+      <c r="I143">
         <v>66227000000</v>
       </c>
-      <c r="J143" s="1"/>
-      <c r="K143" s="1">
+      <c r="K143">
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A144" s="1">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144">
         <v>2017</v>
       </c>
-      <c r="B144" s="1">
+      <c r="B144">
         <v>3</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" t="s">
         <v>7</v>
       </c>
-      <c r="D144" s="1">
+      <c r="D144">
         <v>11060000000</v>
       </c>
-      <c r="E144" s="1">
+      <c r="E144">
         <v>9399000000</v>
       </c>
-      <c r="F144" s="1">
+      <c r="F144">
         <v>9221000000</v>
       </c>
-      <c r="G144" s="1">
+      <c r="G144">
         <v>1178000000</v>
       </c>
-      <c r="H144" s="1">
+      <c r="H144">
         <v>61006000000</v>
       </c>
-      <c r="I144" s="1">
+      <c r="I144">
         <v>70167000000</v>
       </c>
-      <c r="J144" s="1"/>
-      <c r="K144" s="1">
+      <c r="K144">
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A145" s="1">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145">
         <v>2017</v>
       </c>
-      <c r="B145" s="1">
+      <c r="B145">
         <v>4</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" t="s">
         <v>7</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D145">
         <v>10245000000</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E145">
         <v>8501000000</v>
       </c>
-      <c r="F145" s="1">
+      <c r="F145">
         <v>9052000000</v>
       </c>
-      <c r="G145" s="1">
+      <c r="G145">
         <v>572000000</v>
       </c>
-      <c r="H145" s="1">
+      <c r="H145">
         <v>51180000000</v>
       </c>
-      <c r="I145" s="1">
+      <c r="I145">
         <v>60060000000</v>
       </c>
-      <c r="J145" s="1"/>
-      <c r="K145" s="1">
+      <c r="K145">
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A146" s="1">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146">
         <v>2016</v>
       </c>
-      <c r="B146" s="1">
+      <c r="B146">
         <v>1</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" t="s">
         <v>7</v>
       </c>
-      <c r="D146" s="1">
+      <c r="D146">
         <v>9251000000</v>
       </c>
-      <c r="E146" s="1">
+      <c r="E146">
         <v>7762000000</v>
       </c>
-      <c r="F146" s="1">
+      <c r="F146">
         <v>7711000000</v>
       </c>
-      <c r="G146" s="1">
+      <c r="G146">
         <v>946000000</v>
       </c>
-      <c r="H146" s="1">
+      <c r="H146">
         <v>47725000000</v>
       </c>
-      <c r="I146" s="1">
+      <c r="I146">
         <v>58145000000</v>
       </c>
-      <c r="J146" s="1"/>
-      <c r="K146" s="1">
+      <c r="K146">
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A147" s="1">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147">
         <v>2016</v>
       </c>
-      <c r="B147" s="1">
+      <c r="B147">
         <v>2</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" t="s">
         <v>7</v>
       </c>
-      <c r="D147" s="1">
+      <c r="D147">
         <v>10447000000</v>
       </c>
-      <c r="E147" s="1">
+      <c r="E147">
         <v>8970000000</v>
       </c>
-      <c r="F147" s="1">
+      <c r="F147">
         <v>8024000000</v>
       </c>
-      <c r="G147" s="1">
+      <c r="G147">
         <v>1546000000</v>
       </c>
-      <c r="H147" s="1">
+      <c r="H147">
         <v>56415000000</v>
       </c>
-      <c r="I147" s="1">
+      <c r="I147">
         <v>65979000000</v>
       </c>
-      <c r="J147" s="1"/>
-      <c r="K147" s="1">
+      <c r="K147">
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A148" s="1">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148">
         <v>2016</v>
       </c>
-      <c r="B148" s="1">
+      <c r="B148">
         <v>3</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" t="s">
         <v>7</v>
       </c>
-      <c r="D148" s="1">
+      <c r="D148">
         <v>10483000000</v>
       </c>
-      <c r="E148" s="1">
+      <c r="E148">
         <v>9071000000</v>
       </c>
-      <c r="F148" s="1">
+      <c r="F148">
         <v>8514000000</v>
       </c>
-      <c r="G148" s="1">
+      <c r="G148">
         <v>1259000000</v>
       </c>
-      <c r="H148" s="1">
+      <c r="H148">
         <v>58973000000</v>
       </c>
-      <c r="I148" s="1">
+      <c r="I148">
         <v>69028000000</v>
       </c>
-      <c r="J148" s="1"/>
-      <c r="K148" s="1">
+      <c r="K148">
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A149" s="1">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149">
         <v>2016</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149">
         <v>4</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" t="s">
         <v>7</v>
       </c>
-      <c r="D149" s="1">
+      <c r="D149">
         <v>9458000000</v>
       </c>
-      <c r="E149" s="1">
+      <c r="E149">
         <v>7974000000</v>
       </c>
-      <c r="F149" s="1">
+      <c r="F149">
         <v>8438000000</v>
       </c>
-      <c r="G149" s="1">
+      <c r="G149">
         <v>622000000</v>
       </c>
-      <c r="H149" s="1">
+      <c r="H149">
         <v>49985000000</v>
       </c>
-      <c r="I149" s="1">
+      <c r="I149">
         <v>58715000000</v>
       </c>
-      <c r="J149" s="1"/>
-      <c r="K149" s="1">
+      <c r="K149">
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A150" s="1">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150">
         <v>2015</v>
       </c>
-      <c r="B150" s="1">
+      <c r="B150">
         <v>1</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" t="s">
         <v>7</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D150">
         <v>9388000000</v>
       </c>
-      <c r="E150" s="1">
+      <c r="E150">
         <v>7923000000</v>
       </c>
-      <c r="F150" s="1">
+      <c r="F150">
         <v>7990000000</v>
       </c>
-      <c r="G150" s="1">
+      <c r="G150">
         <v>746000000</v>
       </c>
-      <c r="H150" s="1">
+      <c r="H150">
         <v>46221000000</v>
       </c>
-      <c r="I150" s="1">
+      <c r="I150">
         <v>56597000000</v>
       </c>
-      <c r="J150" s="1"/>
-      <c r="K150" s="1">
+      <c r="K150">
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A151" s="1">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151">
         <v>2015</v>
       </c>
-      <c r="B151" s="1">
+      <c r="B151">
         <v>2</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" t="s">
         <v>7</v>
       </c>
-      <c r="D151" s="1">
+      <c r="D151">
         <v>10707000000</v>
       </c>
-      <c r="E151" s="1">
+      <c r="E151">
         <v>9139000000</v>
       </c>
-      <c r="F151" s="1">
+      <c r="F151">
         <v>8233000000</v>
       </c>
-      <c r="G151" s="1">
+      <c r="G151">
         <v>1485000000</v>
       </c>
-      <c r="H151" s="1">
+      <c r="H151">
         <v>54755000000</v>
       </c>
-      <c r="I151" s="1">
+      <c r="I151">
         <v>63937000000</v>
       </c>
-      <c r="J151" s="1"/>
-      <c r="K151" s="1">
+      <c r="K151">
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A152" s="1">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152">
         <v>2015</v>
       </c>
-      <c r="B152" s="1">
+      <c r="B152">
         <v>3</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" t="s">
         <v>7</v>
       </c>
-      <c r="D152" s="1">
+      <c r="D152">
         <v>11107000000</v>
       </c>
-      <c r="E152" s="1">
+      <c r="E152">
         <v>9595000000</v>
       </c>
-      <c r="F152" s="1">
+      <c r="F152">
         <v>8894000000</v>
       </c>
-      <c r="G152" s="1">
+      <c r="G152">
         <v>1315000000</v>
       </c>
-      <c r="H152" s="1">
+      <c r="H152">
         <v>59076000000</v>
       </c>
-      <c r="I152" s="1">
+      <c r="I152">
         <v>68031000000</v>
       </c>
-      <c r="J152" s="1"/>
-      <c r="K152" s="1">
+      <c r="K152">
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A153" s="1">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A153">
         <v>2015</v>
       </c>
-      <c r="B153" s="1">
+      <c r="B153">
         <v>4</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" t="s">
         <v>7</v>
       </c>
-      <c r="D153" s="1">
+      <c r="D153">
         <v>9502000000</v>
       </c>
-      <c r="E153" s="1">
+      <c r="E153">
         <v>8125000000</v>
       </c>
-      <c r="F153" s="1">
+      <c r="F153">
         <v>7785000000</v>
       </c>
-      <c r="G153" s="1">
+      <c r="G153">
         <v>980000000</v>
       </c>
-      <c r="H153" s="1">
+      <c r="H153">
         <v>49573000000</v>
       </c>
-      <c r="I153" s="1">
+      <c r="I153">
         <v>58199000000</v>
       </c>
-      <c r="J153" s="1"/>
-      <c r="K153" s="1">
+      <c r="K153">
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A154" s="1">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A154">
         <v>2014</v>
       </c>
-      <c r="B154" s="1">
+      <c r="B154">
         <v>1</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C154" t="s">
         <v>7</v>
       </c>
-      <c r="D154" s="1">
+      <c r="D154">
         <v>8916000000</v>
       </c>
-      <c r="E154" s="1">
+      <c r="E154">
         <v>7677000000</v>
       </c>
-      <c r="F154" s="1">
+      <c r="F154">
         <v>8296000000</v>
       </c>
-      <c r="G154" s="1">
+      <c r="G154">
         <v>213000000</v>
       </c>
-      <c r="H154" s="1">
+      <c r="H154">
         <v>44601000000</v>
       </c>
-      <c r="I154" s="1">
+      <c r="I154">
         <v>53904000000</v>
       </c>
-      <c r="J154" s="1"/>
-      <c r="K154" s="1">
+      <c r="K154">
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A155" s="1">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155">
         <v>2014</v>
       </c>
-      <c r="B155" s="1">
+      <c r="B155">
         <v>2</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C155" t="s">
         <v>7</v>
       </c>
-      <c r="D155" s="1">
+      <c r="D155">
         <v>10621000000</v>
       </c>
-      <c r="E155" s="1">
+      <c r="E155">
         <v>9266000000</v>
       </c>
-      <c r="F155" s="1">
+      <c r="F155">
         <v>9042000000</v>
       </c>
-      <c r="G155" s="1">
+      <c r="G155">
         <v>801000000</v>
       </c>
-      <c r="H155" s="1">
+      <c r="H155">
         <v>53341000000</v>
       </c>
-      <c r="I155" s="1">
+      <c r="I155">
         <v>61817000000</v>
       </c>
-      <c r="J155" s="1"/>
-      <c r="K155" s="1">
+      <c r="K155">
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A156" s="1">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156">
         <v>2014</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156">
         <v>3</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C156" t="s">
         <v>7</v>
       </c>
-      <c r="D156" s="1">
+      <c r="D156">
         <v>11178000000</v>
       </c>
-      <c r="E156" s="1">
+      <c r="E156">
         <v>9776000000</v>
       </c>
-      <c r="F156" s="1">
+      <c r="F156">
         <v>10343000000</v>
       </c>
-      <c r="G156" s="1">
+      <c r="G156">
         <v>357000000</v>
       </c>
-      <c r="H156" s="1">
+      <c r="H156">
         <v>56955000000</v>
       </c>
-      <c r="I156" s="1">
+      <c r="I156">
         <v>65926000000</v>
       </c>
-      <c r="J156" s="1"/>
-      <c r="K156" s="1">
+      <c r="K156">
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A157" s="1">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157">
         <v>2014</v>
       </c>
-      <c r="B157" s="1">
+      <c r="B157">
         <v>4</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C157" t="s">
         <v>7</v>
       </c>
-      <c r="D157" s="1">
+      <c r="D157">
         <v>9647000000</v>
       </c>
-      <c r="E157" s="1">
+      <c r="E157">
         <v>8235000000</v>
       </c>
-      <c r="F157" s="1">
+      <c r="F157">
         <v>10475000000</v>
       </c>
-      <c r="G157" s="1">
+      <c r="G157">
         <v>-712000000</v>
       </c>
-      <c r="H157" s="1">
+      <c r="H157">
         <v>48028000000</v>
       </c>
-      <c r="I157" s="1">
+      <c r="I157">
         <v>58029000000</v>
       </c>
-      <c r="J157" s="1"/>
-      <c r="K157" s="1">
+      <c r="K157">
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A158" s="1">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158">
         <v>2017</v>
       </c>
-      <c r="B158" s="1">
+      <c r="B158">
         <v>1</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" t="s">
         <v>8</v>
       </c>
-      <c r="D158" s="1">
+      <c r="D158">
         <v>8420000000</v>
       </c>
-      <c r="E158" s="1">
+      <c r="E158">
         <v>7174000000</v>
       </c>
-      <c r="F158" s="1">
+      <c r="F158">
         <v>8142000000</v>
       </c>
-      <c r="G158" s="1">
+      <c r="G158">
         <v>96000000</v>
       </c>
-      <c r="H158" s="1">
+      <c r="H158">
         <v>47611000000</v>
       </c>
-      <c r="I158" s="1">
+      <c r="I158">
         <v>59808000000</v>
       </c>
-      <c r="J158" s="1"/>
-      <c r="K158" s="1">
+      <c r="K158">
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A159" s="1">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159">
         <v>2017</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159">
         <v>2</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" t="s">
         <v>8</v>
       </c>
-      <c r="D159" s="1">
+      <c r="D159">
         <v>10000000000</v>
       </c>
-      <c r="E159" s="1">
+      <c r="E159">
         <v>8622000000</v>
       </c>
-      <c r="F159" s="1">
+      <c r="F159">
         <v>8601000000</v>
       </c>
-      <c r="G159" s="1">
+      <c r="G159">
         <v>818000000</v>
       </c>
-      <c r="H159" s="1">
+      <c r="H159">
         <v>56356000000</v>
       </c>
-      <c r="I159" s="1">
+      <c r="I159">
         <v>67467000000</v>
       </c>
-      <c r="J159" s="1"/>
-      <c r="K159" s="1">
+      <c r="K159">
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A160" s="1">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160">
         <v>2017</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160">
         <v>3</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C160" t="s">
         <v>8</v>
       </c>
-      <c r="D160" s="1">
+      <c r="D160">
         <v>9878000000</v>
       </c>
-      <c r="E160" s="1">
+      <c r="E160">
         <v>8528000000</v>
       </c>
-      <c r="F160" s="1">
+      <c r="F160">
         <v>8786000000</v>
       </c>
-      <c r="G160" s="1">
+      <c r="G160">
         <v>637000000</v>
       </c>
-      <c r="H160" s="1">
+      <c r="H160">
         <v>59145000000</v>
       </c>
-      <c r="I160" s="1">
+      <c r="I160">
         <v>70083000000</v>
       </c>
-      <c r="J160" s="1"/>
-      <c r="K160" s="1">
+      <c r="K160">
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A161" s="1">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161">
         <v>2017</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161">
         <v>4</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C161" t="s">
         <v>8</v>
       </c>
-      <c r="D161" s="1">
+      <c r="D161">
         <v>9438000000</v>
       </c>
-      <c r="E161" s="1">
+      <c r="E161">
         <v>8080000000</v>
       </c>
-      <c r="F161" s="1">
+      <c r="F161">
         <v>8709000000</v>
       </c>
-      <c r="G161" s="1">
+      <c r="G161">
         <v>580000000</v>
       </c>
-      <c r="H161" s="1">
+      <c r="H161">
         <v>53149000000</v>
       </c>
-      <c r="I161" s="1">
+      <c r="I161">
         <v>65028000000</v>
       </c>
-      <c r="J161" s="1"/>
-      <c r="K161" s="1">
+      <c r="K161">
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A162" s="1">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162">
         <v>2016</v>
       </c>
-      <c r="B162" s="1">
+      <c r="B162">
         <v>1</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="C162" t="s">
         <v>8</v>
       </c>
-      <c r="D162" s="1">
+      <c r="D162">
         <v>8195000000</v>
       </c>
-      <c r="E162" s="1">
+      <c r="E162">
         <v>6990000000</v>
       </c>
-      <c r="F162" s="1">
+      <c r="F162">
         <v>7546000000</v>
       </c>
-      <c r="G162" s="1">
+      <c r="G162">
         <v>313000000</v>
       </c>
-      <c r="H162" s="1">
+      <c r="H162">
         <v>46582000000</v>
       </c>
-      <c r="I162" s="1">
+      <c r="I162">
         <v>58273000000</v>
       </c>
-      <c r="J162" s="1"/>
-      <c r="K162" s="1">
+      <c r="K162">
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A163" s="1">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163">
         <v>2016</v>
       </c>
-      <c r="B163" s="1">
+      <c r="B163">
         <v>2</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="C163" t="s">
         <v>8</v>
       </c>
-      <c r="D163" s="1">
+      <c r="D163">
         <v>9396000000</v>
       </c>
-      <c r="E163" s="1">
+      <c r="E163">
         <v>8103000000</v>
       </c>
-      <c r="F163" s="1">
+      <c r="F163">
         <v>8336000000</v>
       </c>
-      <c r="G163" s="1">
+      <c r="G163">
         <v>588000000</v>
       </c>
-      <c r="H163" s="1">
+      <c r="H163">
         <v>54017000000</v>
       </c>
-      <c r="I163" s="1">
+      <c r="I163">
         <v>64725000000</v>
       </c>
-      <c r="J163" s="1"/>
-      <c r="K163" s="1">
+      <c r="K163">
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A164" s="1">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164">
         <v>2016</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164">
         <v>3</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="C164" t="s">
         <v>8</v>
       </c>
-      <c r="D164" s="1">
+      <c r="D164">
         <v>9913000000</v>
       </c>
-      <c r="E164" s="1">
+      <c r="E164">
         <v>8603000000</v>
       </c>
-      <c r="F164" s="1">
+      <c r="F164">
         <v>8289000000</v>
       </c>
-      <c r="G164" s="1">
+      <c r="G164">
         <v>965000000</v>
       </c>
-      <c r="H164" s="1">
+      <c r="H164">
         <v>58172000000</v>
       </c>
-      <c r="I164" s="1">
+      <c r="I164">
         <v>68074000000</v>
       </c>
-      <c r="J164" s="1"/>
-      <c r="K164" s="1">
+      <c r="K164">
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A165" s="1">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165">
         <v>2016</v>
       </c>
-      <c r="B165" s="1">
+      <c r="B165">
         <v>4</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="C165" t="s">
         <v>8</v>
       </c>
-      <c r="D165" s="1">
+      <c r="D165">
         <v>9052000000</v>
       </c>
-      <c r="E165" s="1">
+      <c r="E165">
         <v>7761000000</v>
       </c>
-      <c r="F165" s="1">
+      <c r="F165">
         <v>8047000000</v>
       </c>
-      <c r="G165" s="1">
+      <c r="G165">
         <v>397000000</v>
       </c>
-      <c r="H165" s="1">
+      <c r="H165">
         <v>51538000000</v>
       </c>
-      <c r="I165" s="1">
+      <c r="I165">
         <v>62518000000</v>
       </c>
-      <c r="J165" s="1"/>
-      <c r="K165" s="1">
+      <c r="K165">
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A166" s="1">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166">
         <v>2015</v>
       </c>
-      <c r="B166" s="1">
+      <c r="B166">
         <v>1</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="C166" t="s">
         <v>8</v>
       </c>
-      <c r="D166" s="1">
+      <c r="D166">
         <v>8608000000</v>
       </c>
-      <c r="E166" s="1">
+      <c r="E166">
         <v>7420000000</v>
       </c>
-      <c r="F166" s="1">
+      <c r="F166">
         <v>7867000000</v>
       </c>
-      <c r="G166" s="1">
+      <c r="G166">
         <v>508000000</v>
       </c>
-      <c r="H166" s="1">
+      <c r="H166">
         <v>46444000000</v>
       </c>
-      <c r="I166" s="1">
+      <c r="I166">
         <v>57269000000</v>
       </c>
-      <c r="J166" s="1"/>
-      <c r="K166" s="1">
+      <c r="K166">
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A167" s="1">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167">
         <v>2015</v>
       </c>
-      <c r="B167" s="1">
+      <c r="B167">
         <v>2</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C167" t="s">
         <v>8</v>
       </c>
-      <c r="D167" s="1">
+      <c r="D167">
         <v>9914000000</v>
       </c>
-      <c r="E167" s="1">
+      <c r="E167">
         <v>8676000000</v>
       </c>
-      <c r="F167" s="1">
+      <c r="F167">
         <v>8469000000</v>
       </c>
-      <c r="G167" s="1">
+      <c r="G167">
         <v>1193000000</v>
       </c>
-      <c r="H167" s="1">
+      <c r="H167">
         <v>54289000000</v>
       </c>
-      <c r="I167" s="1">
+      <c r="I167">
         <v>64685000000</v>
       </c>
-      <c r="J167" s="1"/>
-      <c r="K167" s="1">
+      <c r="K167">
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A168" s="1">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A168">
         <v>2015</v>
       </c>
-      <c r="B168" s="1">
+      <c r="B168">
         <v>3</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C168" t="s">
         <v>8</v>
       </c>
-      <c r="D168" s="1">
+      <c r="D168">
         <v>10306000000</v>
       </c>
-      <c r="E168" s="1">
+      <c r="E168">
         <v>8960000000</v>
       </c>
-      <c r="F168" s="1">
+      <c r="F168">
         <v>8407000000</v>
       </c>
-      <c r="G168" s="1">
+      <c r="G168">
         <v>4816000000</v>
       </c>
-      <c r="H168" s="1">
+      <c r="H168">
         <v>57160000000</v>
       </c>
-      <c r="I168" s="1">
+      <c r="I168">
         <v>66745000000</v>
       </c>
-      <c r="J168" s="1"/>
-      <c r="K168" s="1">
+      <c r="K168">
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A169" s="1">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169">
         <v>2015</v>
       </c>
-      <c r="B169" s="1">
+      <c r="B169">
         <v>4</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C169" t="s">
         <v>8</v>
       </c>
-      <c r="D169" s="1">
+      <c r="D169">
         <v>9036000000</v>
       </c>
-      <c r="E169" s="1">
+      <c r="E169">
         <v>7729000000</v>
       </c>
-      <c r="F169" s="1">
+      <c r="F169">
         <v>7955000000</v>
       </c>
-      <c r="G169" s="1">
+      <c r="G169">
         <v>823000000</v>
       </c>
-      <c r="H169" s="1">
+      <c r="H169">
         <v>50718000000</v>
       </c>
-      <c r="I169" s="1">
+      <c r="I169">
         <v>61304000000</v>
       </c>
-      <c r="J169" s="1"/>
-      <c r="K169" s="1">
+      <c r="K169">
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A170" s="1">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170">
         <v>2014</v>
       </c>
-      <c r="B170" s="1">
+      <c r="B170">
         <v>1</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C170" t="s">
         <v>8</v>
       </c>
-      <c r="D170" s="1">
+      <c r="D170">
         <v>8696000000</v>
       </c>
-      <c r="E170" s="1">
+      <c r="E170">
         <v>7384000000</v>
       </c>
-      <c r="F170" s="1">
+      <c r="F170">
         <v>9045000000</v>
       </c>
-      <c r="G170" s="1">
+      <c r="G170">
         <v>-609000000</v>
       </c>
-      <c r="H170" s="1">
+      <c r="H170">
         <v>46383000000</v>
       </c>
-      <c r="I170" s="1">
+      <c r="I170">
         <v>57216000000</v>
       </c>
-      <c r="J170" s="1"/>
-      <c r="K170" s="1">
+      <c r="K170">
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A171" s="1">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171">
         <v>2014</v>
       </c>
-      <c r="B171" s="1">
+      <c r="B171">
         <v>2</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="C171" t="s">
         <v>8</v>
       </c>
-      <c r="D171" s="1">
+      <c r="D171">
         <v>10329000000</v>
       </c>
-      <c r="E171" s="1">
+      <c r="E171">
         <v>8981000000</v>
       </c>
-      <c r="F171" s="1">
+      <c r="F171">
         <v>9423000000</v>
       </c>
-      <c r="G171" s="1">
+      <c r="G171">
         <v>789000000</v>
       </c>
-      <c r="H171" s="1">
+      <c r="H171">
         <v>53900000000</v>
       </c>
-      <c r="I171" s="1">
+      <c r="I171">
         <v>63214000000</v>
       </c>
-      <c r="J171" s="1"/>
-      <c r="K171" s="1">
+      <c r="K171">
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A172" s="1">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172">
         <v>2014</v>
       </c>
-      <c r="B172" s="1">
+      <c r="B172">
         <v>3</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="C172" t="s">
         <v>8</v>
       </c>
-      <c r="D172" s="1">
+      <c r="D172">
         <v>10563000000</v>
       </c>
-      <c r="E172" s="1">
+      <c r="E172">
         <v>9314000000</v>
       </c>
-      <c r="F172" s="1">
+      <c r="F172">
         <v>9372000000</v>
       </c>
-      <c r="G172" s="1">
+      <c r="G172">
         <v>924000000</v>
       </c>
-      <c r="H172" s="1">
+      <c r="H172">
         <v>56065000000</v>
       </c>
-      <c r="I172" s="1">
+      <c r="I172">
         <v>65378000000</v>
       </c>
-      <c r="J172" s="1"/>
-      <c r="K172" s="1">
+      <c r="K172">
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A173" s="1">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173">
         <v>2014</v>
       </c>
-      <c r="B173" s="1">
+      <c r="B173">
         <v>4</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="C173" t="s">
         <v>8</v>
       </c>
-      <c r="D173" s="1">
+      <c r="D173">
         <v>9313000000</v>
       </c>
-      <c r="E173" s="1">
+      <c r="E173">
         <v>8083000000</v>
       </c>
-      <c r="F173" s="1">
+      <c r="F173">
         <v>8688000000</v>
       </c>
-      <c r="G173" s="1">
+      <c r="G173">
         <v>28000000</v>
       </c>
-      <c r="H173" s="1">
+      <c r="H173">
         <v>49211000000</v>
       </c>
-      <c r="I173" s="1">
+      <c r="I173">
         <v>60213000000</v>
       </c>
-      <c r="J173" s="1"/>
-      <c r="K173" s="1">
+      <c r="K173">
         <v>54000000</v>
       </c>
     </row>
@@ -6693,13 +6643,13 @@
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6716,7 +6666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -6733,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -6750,7 +6700,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -6767,7 +6717,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -6784,7 +6734,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -6801,7 +6751,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -6818,7 +6768,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -6835,7 +6785,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -6852,7 +6802,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -6869,7 +6819,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -6886,7 +6836,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -6903,7 +6853,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -6920,7 +6870,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -6937,7 +6887,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -6954,7 +6904,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -6971,7 +6921,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -6988,7 +6938,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7005,7 +6955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7022,7 +6972,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7039,7 +6989,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7056,7 +7006,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7073,7 +7023,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7090,7 +7040,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7107,7 +7057,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2020</v>
       </c>

</xml_diff>

<commit_message>
updated the share repurchase tab to reflect the effect from shares sales made to raise cash during covid
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49AE8822-1526-4537-8620-2DD0DDB42906}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED53E36C-7C69-483A-AB6E-4E62641CE550}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
     <sheet name="share_repurchases" sheetId="3" r:id="rId2"/>
+    <sheet name="share_sales" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Proceeds</t>
+  </si>
+  <si>
+    <t>Shares Sold</t>
   </si>
 </sst>
 </file>
@@ -571,8 +578,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -954,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O125" sqref="O125"/>
     </sheetView>
   </sheetViews>
@@ -6640,7 +6648,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,4 +7085,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490D347E-B079-4188-B046-54C6AF8BB324}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>143597509</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1901355562.5899999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2021</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>79599019</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1082205377.28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>6500000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>158535000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>2100000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>83433000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>69338841</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2293578491.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2021</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>14200000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>685282000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix incorrect entry for DAL 2022Q4 passenger revenue. minor changes to wording in About.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED53E36C-7C69-483A-AB6E-4E62641CE550}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D780C85F-1288-42BC-88C9-6CABC16602D3}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K173"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O125" sqref="O125"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3304,7 +3304,7 @@
         <v>13435000000</v>
       </c>
       <c r="E72">
-        <v>13435000000</v>
+        <v>10889000000</v>
       </c>
       <c r="F72">
         <v>11965000000</v>
@@ -7091,7 +7091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490D347E-B079-4188-B046-54C6AF8BB324}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add DAL 2024Q4 and 2024FY results. Fix handling of period comparison tables and percent difference comparison.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D780C85F-1288-42BC-88C9-6CABC16602D3}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33B676AA-ACB6-4E05-94D7-BB389D1BBF6D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="180" yWindow="1275" windowWidth="28695" windowHeight="15240" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -960,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
-  <dimension ref="A1:K173"/>
+  <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6636,6 +6636,136 @@
       </c>
       <c r="K173">
         <v>54000000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>2024</v>
+      </c>
+      <c r="B174">
+        <v>4</v>
+      </c>
+      <c r="C174" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174">
+        <v>15559000000</v>
+      </c>
+      <c r="E174">
+        <v>12815000000</v>
+      </c>
+      <c r="F174">
+        <v>13842000000</v>
+      </c>
+      <c r="G174">
+        <v>843000000</v>
+      </c>
+      <c r="H174">
+        <v>60387000000</v>
+      </c>
+      <c r="I174">
+        <v>72035000000</v>
+      </c>
+      <c r="K174">
+        <v>425000000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>2024</v>
+      </c>
+      <c r="B175" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175">
+        <v>61643000000</v>
+      </c>
+      <c r="E175">
+        <v>50894000000</v>
+      </c>
+      <c r="F175">
+        <v>55648000000</v>
+      </c>
+      <c r="G175">
+        <v>3457000000</v>
+      </c>
+      <c r="H175">
+        <v>246145000000</v>
+      </c>
+      <c r="I175">
+        <v>288394000000</v>
+      </c>
+      <c r="K175">
+        <v>1389000000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>2024</v>
+      </c>
+      <c r="B176">
+        <v>4</v>
+      </c>
+      <c r="C176" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>2024</v>
+      </c>
+      <c r="B177" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2024</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>2024</v>
+      </c>
+      <c r="B179" t="s">
+        <v>9</v>
+      </c>
+      <c r="C179" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>2024</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="C180" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>2024</v>
+      </c>
+      <c r="B181" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added UAL 2024Q4 and 2024FY results
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33B676AA-ACB6-4E05-94D7-BB389D1BBF6D}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90C73CE5-0F1B-4C34-B9DD-DD1013AAFE3F}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1275" windowWidth="28695" windowHeight="15240" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K178" sqref="K178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6712,8 +6712,29 @@
       <c r="C176" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176">
+        <v>14695000000</v>
+      </c>
+      <c r="E176">
+        <v>13275000000</v>
+      </c>
+      <c r="F176">
+        <v>13192000000</v>
+      </c>
+      <c r="G176">
+        <v>985000000</v>
+      </c>
+      <c r="H176">
+        <v>64463000000</v>
+      </c>
+      <c r="I176">
+        <v>78298000000</v>
+      </c>
+      <c r="K176">
+        <v>294000000</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6723,8 +6744,29 @@
       <c r="C177" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177">
+        <v>57063000000</v>
+      </c>
+      <c r="E177">
+        <v>51829000000</v>
+      </c>
+      <c r="F177">
+        <v>51967000000</v>
+      </c>
+      <c r="G177">
+        <v>3149000000</v>
+      </c>
+      <c r="H177">
+        <v>258503000000</v>
+      </c>
+      <c r="I177">
+        <v>311185000000</v>
+      </c>
+      <c r="K177">
+        <v>713000000</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6735,7 +6777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6746,7 +6788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6757,7 +6799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2024</v>
       </c>

</xml_diff>

<commit_message>
Added AAL 2024Q4 and 2024FY results (except profit sharing which was not reported and will need to wait for 10K)
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90C73CE5-0F1B-4C34-B9DD-DD1013AAFE3F}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF2F9828-4E7D-4ED2-8496-4CA91ED96770}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -962,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K178" sqref="K178"/>
     </sheetView>
   </sheetViews>
@@ -6776,6 +6776,24 @@
       <c r="C178" t="s">
         <v>6</v>
       </c>
+      <c r="D178">
+        <v>13660000000</v>
+      </c>
+      <c r="E178">
+        <v>12402000000</v>
+      </c>
+      <c r="F178">
+        <v>12526000000</v>
+      </c>
+      <c r="G178">
+        <v>590000000</v>
+      </c>
+      <c r="H178">
+        <v>60676000000</v>
+      </c>
+      <c r="I178">
+        <v>71503000000</v>
+      </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
@@ -6786,6 +6804,24 @@
       </c>
       <c r="C179" t="s">
         <v>6</v>
+      </c>
+      <c r="D179">
+        <v>54211000000</v>
+      </c>
+      <c r="E179">
+        <v>49586000000</v>
+      </c>
+      <c r="F179">
+        <v>51597000000</v>
+      </c>
+      <c r="G179">
+        <v>846000000</v>
+      </c>
+      <c r="H179">
+        <v>248795000000</v>
+      </c>
+      <c r="I179">
+        <v>292948000000</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added LUV 2024Q4 and 2024FY results
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF2F9828-4E7D-4ED2-8496-4CA91ED96770}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F586315B-5B2B-40EE-B5AE-0C7371837CF6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K178" sqref="K178"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J182" sqref="J182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6834,6 +6834,27 @@
       <c r="C180" t="s">
         <v>15</v>
       </c>
+      <c r="D180">
+        <v>6931000000</v>
+      </c>
+      <c r="E180">
+        <v>6307000000</v>
+      </c>
+      <c r="F180">
+        <v>6653000000</v>
+      </c>
+      <c r="G180">
+        <v>261000000</v>
+      </c>
+      <c r="H180">
+        <v>34471000000</v>
+      </c>
+      <c r="I180">
+        <v>43533000000</v>
+      </c>
+      <c r="K180">
+        <v>54000000</v>
+      </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
@@ -6844,6 +6865,30 @@
       </c>
       <c r="C181" t="s">
         <v>15</v>
+      </c>
+      <c r="D181">
+        <v>27483000000</v>
+      </c>
+      <c r="E181">
+        <v>24980000000</v>
+      </c>
+      <c r="F181">
+        <v>27162000000</v>
+      </c>
+      <c r="G181">
+        <v>465000000</v>
+      </c>
+      <c r="H181">
+        <v>142515000000</v>
+      </c>
+      <c r="I181">
+        <v>177250000000</v>
+      </c>
+      <c r="J181">
+        <v>5069000000</v>
+      </c>
+      <c r="K181">
+        <v>103000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DAL 2024 long term debt from 10K
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F586315B-5B2B-40EE-B5AE-0C7371837CF6}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62378EFC-0109-489F-B81D-B608561648A6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -962,24 +962,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J182" sqref="J182"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J176" sqref="J176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6698,11 +6698,14 @@
       <c r="I175">
         <v>288394000000</v>
       </c>
+      <c r="J175">
+        <v>13546000000</v>
+      </c>
       <c r="K175">
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6734,7 +6737,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6766,7 +6769,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6795,7 +6798,7 @@
         <v>71503000000</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6824,7 +6827,7 @@
         <v>292948000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6856,7 +6859,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6904,13 +6907,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6927,7 +6930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -6944,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -6961,7 +6964,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -6978,7 +6981,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -6995,7 +6998,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7012,7 +7015,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7029,7 +7032,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7046,7 +7049,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7063,7 +7066,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7080,7 +7083,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7097,7 +7100,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7114,7 +7117,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7131,7 +7134,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7148,7 +7151,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7165,7 +7168,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7182,7 +7185,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7199,7 +7202,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7216,7 +7219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7233,7 +7236,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7250,7 +7253,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7284,7 +7287,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7318,7 +7321,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7348,16 +7351,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7374,7 +7377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -7391,7 +7394,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -7408,7 +7411,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7425,7 +7428,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7442,7 +7445,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -7459,7 +7462,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
add AAL 2024 long term debt and profit sharing from 10K
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62378EFC-0109-489F-B81D-B608561648A6}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85657B72-BDE6-4CE4-BF05-150728504D56}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -963,23 +963,24 @@
   <dimension ref="A1:K181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J176" sqref="J176"/>
+      <selection activeCell="P182" sqref="P182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1078,7 +1079,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1206,7 +1207,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1302,7 +1303,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1922,7 +1923,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2056,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2120,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2152,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2184,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2216,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2481,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2609,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2833,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2970,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3002,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3130,7 +3131,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3354,7 +3355,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3389,7 +3390,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3424,7 +3425,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3459,7 +3460,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3491,7 +3492,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3523,7 +3524,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3619,7 +3620,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3715,7 +3716,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3747,7 +3748,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3779,7 +3780,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3878,7 +3879,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3948,7 +3949,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3977,10 +3978,11 @@
         <v>70516000000</v>
       </c>
       <c r="K92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+        <f>ROUND($K$179*((D92-F92)/($D$179-$F$179)),-5)</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4012,7 +4014,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4073,10 +4075,11 @@
         <v>75263000000</v>
       </c>
       <c r="K95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+        <f>ROUND($K$179*((D95-F95)/($D$179-$F$179)),-5)</f>
+        <v>120700000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4140,7 +4143,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4169,10 +4172,11 @@
         <v>75665000000</v>
       </c>
       <c r="K98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+        <f>ROUND($K$179*((D98-F98)/($D$179-$F$179)),-5)</f>
+        <v>7800000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4204,7 +4208,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4236,7 +4240,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4271,7 +4275,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4306,7 +4310,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4341,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4376,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4411,7 +4415,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4446,7 +4450,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4481,7 +4485,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4516,7 +4520,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4551,7 +4555,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4586,7 +4590,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4621,7 +4625,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4656,7 +4660,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4691,7 +4695,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4726,7 +4730,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4761,7 +4765,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4796,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4831,7 +4835,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4866,7 +4870,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4901,7 +4905,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4936,7 +4940,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4971,7 +4975,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5006,7 +5010,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5038,7 +5042,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5070,7 +5074,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5102,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5134,7 +5138,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5166,7 +5170,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5198,7 +5202,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5230,7 +5234,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5262,7 +5266,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5294,7 +5298,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5326,7 +5330,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5358,7 +5362,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5390,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5422,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5454,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5486,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5518,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5550,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5582,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5614,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5646,7 +5650,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5678,7 +5682,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5710,7 +5714,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5742,7 +5746,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5774,7 +5778,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5806,7 +5810,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5838,7 +5842,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5870,7 +5874,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5902,7 +5906,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5934,7 +5938,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5966,7 +5970,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -5998,7 +6002,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6030,7 +6034,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6062,7 +6066,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6094,7 +6098,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6126,7 +6130,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6158,7 +6162,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6190,7 +6194,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6222,7 +6226,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6254,7 +6258,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6286,7 +6290,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6318,7 +6322,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6350,7 +6354,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6382,7 +6386,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6414,7 +6418,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6446,7 +6450,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6478,7 +6482,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6510,7 +6514,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6542,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6574,7 +6578,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6606,7 +6610,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6638,7 +6642,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6670,7 +6674,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6705,7 +6709,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6737,7 +6741,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6769,7 +6773,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6797,8 +6801,12 @@
       <c r="I178">
         <v>71503000000</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K178">
+        <f>ROUND($K$179*((D178-F178)/($D$179-$F$179)),-5)</f>
+        <v>98900000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6826,8 +6834,14 @@
       <c r="I179">
         <v>292948000000</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J179">
+        <v>24617000000</v>
+      </c>
+      <c r="K179">
+        <v>228000000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6859,7 +6873,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6907,13 +6921,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6930,7 +6944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -6947,7 +6961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -6964,7 +6978,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -6981,7 +6995,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -6998,7 +7012,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7015,7 +7029,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7032,7 +7046,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7049,7 +7063,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7066,7 +7080,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7083,7 +7097,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7100,7 +7114,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7117,7 +7131,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7134,7 +7148,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7151,7 +7165,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7168,7 +7182,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7185,7 +7199,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7202,7 +7216,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7219,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7236,7 +7250,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7253,7 +7267,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7270,7 +7284,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7287,7 +7301,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7304,7 +7318,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7321,7 +7335,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7351,16 +7365,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7377,7 +7391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -7394,7 +7408,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -7411,7 +7425,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7428,7 +7442,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7445,7 +7459,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -7462,7 +7476,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
correct table formatting for dollar metrics
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85657B72-BDE6-4CE4-BF05-150728504D56}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0DCD385-305D-4216-834C-461474CECC45}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P182" sqref="P182"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K101" sqref="K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3978,8 +3978,8 @@
         <v>70516000000</v>
       </c>
       <c r="K92">
-        <f>ROUND($K$179*((D92-F92)/($D$179-$F$179)),-5)</f>
-        <v>600000</v>
+        <f>ROUND($K$179*((D92-F92)/($D$179-$F$179)),0)</f>
+        <v>610559</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -4075,8 +4075,8 @@
         <v>75263000000</v>
       </c>
       <c r="K95">
-        <f>ROUND($K$179*((D95-F95)/($D$179-$F$179)),-5)</f>
-        <v>120700000</v>
+        <f>ROUND($K$179*((D95-F95)/($D$179-$F$179)),0)</f>
+        <v>120716144</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -4172,8 +4172,8 @@
         <v>75665000000</v>
       </c>
       <c r="K98">
-        <f>ROUND($K$179*((D98-F98)/($D$179-$F$179)),-5)</f>
-        <v>7800000</v>
+        <f>ROUND($K$179*((D98-F98)/($D$179-$F$179)),0)</f>
+        <v>7762816</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -6802,8 +6802,8 @@
         <v>71503000000</v>
       </c>
       <c r="K178">
-        <f>ROUND($K$179*((D178-F178)/($D$179-$F$179)),-5)</f>
-        <v>98900000</v>
+        <f>ROUND($K$179*((D178-F178)/($D$179-$F$179)),0)</f>
+        <v>98910482</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add UAL 2024 long term debt from 10K
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0DCD385-305D-4216-834C-461474CECC45}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6DB6F45-BF2A-4D81-860A-FE1E94430995}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -962,25 +962,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K177" sqref="K177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>610559</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>120716144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>7762816</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6769,11 +6769,14 @@
       <c r="I177">
         <v>311185000000</v>
       </c>
+      <c r="J177">
+        <v>21680000000</v>
+      </c>
       <c r="K177">
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6806,7 +6809,7 @@
         <v>98910482</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6841,7 +6844,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6873,7 +6876,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6921,13 +6924,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6944,7 +6947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -6961,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -6978,7 +6981,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -6995,7 +6998,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -7012,7 +7015,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7029,7 +7032,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7046,7 +7049,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7063,7 +7066,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7080,7 +7083,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7097,7 +7100,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7114,7 +7117,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7131,7 +7134,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7148,7 +7151,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7165,7 +7168,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7182,7 +7185,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7199,7 +7202,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7216,7 +7219,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7233,7 +7236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7250,7 +7253,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7284,7 +7287,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7318,7 +7321,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7335,7 +7338,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7365,16 +7368,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7391,7 +7394,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -7408,7 +7411,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -7425,7 +7428,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7442,7 +7445,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7459,7 +7462,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -7476,7 +7479,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
Add DAL 2025Q1 results.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6DB6F45-BF2A-4D81-860A-FE1E94430995}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98D61744-1AD1-4742-81B9-31A82AA82897}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -960,27 +960,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
-  <dimension ref="A1:K181"/>
+  <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K177" sqref="K177"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K183" sqref="K183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>610559</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>120716144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>7762816</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>98910482</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6909,6 +6909,71 @@
       </c>
       <c r="K181">
         <v>103000000</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>2025</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182">
+        <v>14040000000</v>
+      </c>
+      <c r="E182">
+        <v>11480000000</v>
+      </c>
+      <c r="F182">
+        <v>13471000000</v>
+      </c>
+      <c r="G182">
+        <v>240000000</v>
+      </c>
+      <c r="H182">
+        <v>55678000000</v>
+      </c>
+      <c r="I182">
+        <v>68401000000</v>
+      </c>
+      <c r="K182">
+        <v>124000000</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>2025</v>
+      </c>
+      <c r="B183">
+        <v>1</v>
+      </c>
+      <c r="C183" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>2025</v>
+      </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>2025</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="C185" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -6924,13 +6989,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6947,7 +7012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -6964,7 +7029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -6981,7 +7046,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -6998,7 +7063,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -7015,7 +7080,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7032,7 +7097,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7049,7 +7114,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7066,7 +7131,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7083,7 +7148,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7100,7 +7165,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7117,7 +7182,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7134,7 +7199,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7151,7 +7216,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7168,7 +7233,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7185,7 +7250,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7202,7 +7267,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7219,7 +7284,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7236,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7253,7 +7318,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7270,7 +7335,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7287,7 +7352,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7304,7 +7369,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7321,7 +7386,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7338,7 +7403,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7368,16 +7433,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7394,7 +7459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -7411,7 +7476,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -7428,7 +7493,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7445,7 +7510,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7462,7 +7527,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -7479,7 +7544,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
Add UAL, AAL, LUV 2025Q1 results.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98D61744-1AD1-4742-81B9-31A82AA82897}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52B9C01-43C3-47D3-B33B-5631F6EBE06B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K183" sqref="K183"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J188" sqref="J188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,7 +4043,7 @@
         <v>71668000000</v>
       </c>
       <c r="K94">
-        <v>0</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -6953,6 +6953,27 @@
       <c r="C183" t="s">
         <v>8</v>
       </c>
+      <c r="D183">
+        <v>13213000000</v>
+      </c>
+      <c r="E183">
+        <v>11860000000</v>
+      </c>
+      <c r="F183">
+        <v>12605000000</v>
+      </c>
+      <c r="G183">
+        <v>387000000</v>
+      </c>
+      <c r="H183">
+        <v>59517000000</v>
+      </c>
+      <c r="I183">
+        <v>75155000000</v>
+      </c>
+      <c r="K183">
+        <v>43000000</v>
+      </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
@@ -6964,6 +6985,27 @@
       <c r="C184" t="s">
         <v>6</v>
       </c>
+      <c r="D184">
+        <v>12551000000</v>
+      </c>
+      <c r="E184">
+        <v>11391000000</v>
+      </c>
+      <c r="F184">
+        <v>12821000000</v>
+      </c>
+      <c r="G184">
+        <v>-473000000</v>
+      </c>
+      <c r="H184">
+        <v>56356000000</v>
+      </c>
+      <c r="I184">
+        <v>69904000000</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
@@ -6974,6 +7016,27 @@
       </c>
       <c r="C185" t="s">
         <v>15</v>
+      </c>
+      <c r="D185">
+        <v>6428000000</v>
+      </c>
+      <c r="E185">
+        <v>5811000000</v>
+      </c>
+      <c r="F185">
+        <v>6651000000</v>
+      </c>
+      <c r="G185">
+        <v>-149000000</v>
+      </c>
+      <c r="H185">
+        <v>30629000000</v>
+      </c>
+      <c r="I185">
+        <v>41432000000</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6986,7 +7049,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add 2025Q2 results for DAL and UAL
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="284" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52B9C01-43C3-47D3-B33B-5631F6EBE06B}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8EA499F-82C8-4305-9EDE-866F68DE8AA9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -960,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
-  <dimension ref="A1:K185"/>
+  <dimension ref="A1:K189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J188" sqref="J188"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F192" sqref="F192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7037,6 +7037,92 @@
       </c>
       <c r="K185">
         <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>2025</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186" t="s">
+        <v>7</v>
+      </c>
+      <c r="D186">
+        <v>16648000000</v>
+      </c>
+      <c r="E186">
+        <v>13867000000</v>
+      </c>
+      <c r="F186">
+        <v>14546000000</v>
+      </c>
+      <c r="G186">
+        <v>2130000000</v>
+      </c>
+      <c r="H186">
+        <v>66417000000</v>
+      </c>
+      <c r="I186">
+        <v>77645000000</v>
+      </c>
+      <c r="K186">
+        <v>470000000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>2025</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
+        <v>8</v>
+      </c>
+      <c r="D187">
+        <v>15236000000</v>
+      </c>
+      <c r="E187">
+        <v>13836000000</v>
+      </c>
+      <c r="F187">
+        <v>13911000000</v>
+      </c>
+      <c r="G187">
+        <v>973000000</v>
+      </c>
+      <c r="H187">
+        <v>70088000000</v>
+      </c>
+      <c r="I187">
+        <v>84347000000</v>
+      </c>
+      <c r="K187">
+        <v>188000000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>2025</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>2025</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add DAL 2025Q3 results.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E95FC9B8-0AC5-477A-AA0D-6848D3894B51}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F0D4930-3EC2-41C2-B483-06C337C24918}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -639,10 +639,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -960,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
-  <dimension ref="A1:K189"/>
+  <dimension ref="A1:K193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G189" sqref="G189"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H191" sqref="H191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7162,6 +7158,71 @@
       </c>
       <c r="K189">
         <v>14000000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2025</v>
+      </c>
+      <c r="B190">
+        <v>3</v>
+      </c>
+      <c r="C190" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190">
+        <v>16673000000</v>
+      </c>
+      <c r="E190">
+        <v>13506000000</v>
+      </c>
+      <c r="F190">
+        <v>14989000000</v>
+      </c>
+      <c r="G190">
+        <v>1417000000</v>
+      </c>
+      <c r="H190">
+        <v>67621000000</v>
+      </c>
+      <c r="I190">
+        <v>79054000000</v>
+      </c>
+      <c r="K190">
+        <v>392000000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>2025</v>
+      </c>
+      <c r="B191">
+        <v>3</v>
+      </c>
+      <c r="C191" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>2025</v>
+      </c>
+      <c r="B192">
+        <v>3</v>
+      </c>
+      <c r="C192" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>2025</v>
+      </c>
+      <c r="B193">
+        <v>3</v>
+      </c>
+      <c r="C193" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add UAL 2025Q3 results
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="343" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F0D4930-3EC2-41C2-B483-06C337C24918}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43695330-E299-43EC-92E4-BADFF45452BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -639,6 +639,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -958,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H191" sqref="H191"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G192" sqref="G192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7201,6 +7205,27 @@
       </c>
       <c r="C191" t="s">
         <v>8</v>
+      </c>
+      <c r="D191">
+        <v>15225000000</v>
+      </c>
+      <c r="E191">
+        <v>13815000000</v>
+      </c>
+      <c r="F191">
+        <v>13830000000</v>
+      </c>
+      <c r="G191">
+        <v>949000000</v>
+      </c>
+      <c r="H191">
+        <v>73769000000</v>
+      </c>
+      <c r="I191">
+        <v>87417000000</v>
+      </c>
+      <c r="K191">
+        <v>228000000</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add LUV 2025Q3 results.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="351" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43695330-E299-43EC-92E4-BADFF45452BF}"/>
+  <xr:revisionPtr revIDLastSave="358" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD6E3C52-A0F7-4849-918C-15B03A8EB719}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G192" sqref="G192"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L201" sqref="L201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7239,7 +7239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>2025</v>
       </c>
@@ -7248,6 +7248,27 @@
       </c>
       <c r="C193" t="s">
         <v>15</v>
+      </c>
+      <c r="D193">
+        <v>6949000000</v>
+      </c>
+      <c r="E193">
+        <v>6313000000</v>
+      </c>
+      <c r="F193">
+        <v>6914000000</v>
+      </c>
+      <c r="G193">
+        <v>54000000</v>
+      </c>
+      <c r="H193">
+        <v>36362000000</v>
+      </c>
+      <c r="I193">
+        <v>45567000000</v>
+      </c>
+      <c r="K193">
+        <v>11000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add AAL 2025Q3 results.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD6E3C52-A0F7-4849-918C-15B03A8EB719}"/>
+  <xr:revisionPtr revIDLastSave="365" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E149F9C-2E14-4D5E-8455-3FFCC444FE04}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L201" sqref="L201"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K193" sqref="K193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7237,6 +7237,27 @@
       </c>
       <c r="C192" t="s">
         <v>6</v>
+      </c>
+      <c r="D192">
+        <v>13691000000</v>
+      </c>
+      <c r="E192">
+        <v>12471000000</v>
+      </c>
+      <c r="F192">
+        <v>13540000000</v>
+      </c>
+      <c r="G192">
+        <v>-114000000</v>
+      </c>
+      <c r="H192">
+        <v>66580000000</v>
+      </c>
+      <c r="I192">
+        <v>77400000000</v>
+      </c>
+      <c r="K192">
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes to the SEC scraping and prep pipelines as well as the gitignore file to clean up file output and storage. Adds DAL Q4 and FY 2025 results except for long term debt. Adds DAL Q4 2025 insights. Remaining DAL FY result and insights awaiting release of 10-K.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E149F9C-2E14-4D5E-8455-3FFCC444FE04}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{180469F5-A0EE-40E9-991D-66A7579DB96B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -960,27 +960,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
-  <dimension ref="A1:K193"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K193" sqref="K193"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G194" sqref="G194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>610559</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>120716144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>7762816</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>98910482</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>2025</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>124000000</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2025</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>2025</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2025</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2025</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>470000000</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2025</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2025</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>77636000000</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2025</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2025</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>392000000</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2025</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2025</v>
       </c>
@@ -7260,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2025</v>
       </c>
@@ -7290,6 +7290,136 @@
       </c>
       <c r="K193">
         <v>11000000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>2025</v>
+      </c>
+      <c r="B194">
+        <v>4</v>
+      </c>
+      <c r="C194" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194">
+        <v>16003000000</v>
+      </c>
+      <c r="E194">
+        <v>12916000000</v>
+      </c>
+      <c r="F194">
+        <v>14536000000</v>
+      </c>
+      <c r="G194">
+        <v>1219000000</v>
+      </c>
+      <c r="H194">
+        <v>59861000000</v>
+      </c>
+      <c r="I194">
+        <v>72946000000</v>
+      </c>
+      <c r="K194">
+        <v>351000000</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>2025</v>
+      </c>
+      <c r="B195" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195">
+        <v>63364000000</v>
+      </c>
+      <c r="E195">
+        <v>51768000000</v>
+      </c>
+      <c r="F195">
+        <v>57542000000</v>
+      </c>
+      <c r="G195">
+        <v>5005000000</v>
+      </c>
+      <c r="H195">
+        <v>249578000000</v>
+      </c>
+      <c r="I195">
+        <v>298045000000</v>
+      </c>
+      <c r="K195">
+        <v>1337000000</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>2025</v>
+      </c>
+      <c r="B196">
+        <v>4</v>
+      </c>
+      <c r="C196" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>2025</v>
+      </c>
+      <c r="B197" t="s">
+        <v>9</v>
+      </c>
+      <c r="C197" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>2025</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+      <c r="C198" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>2025</v>
+      </c>
+      <c r="B199" t="s">
+        <v>9</v>
+      </c>
+      <c r="C199" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>2025</v>
+      </c>
+      <c r="B200">
+        <v>4</v>
+      </c>
+      <c r="C200" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>2025</v>
+      </c>
+      <c r="B201" t="s">
+        <v>9</v>
+      </c>
+      <c r="C201" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -7305,13 +7435,13 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7328,7 +7458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -7345,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -7362,7 +7492,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -7379,7 +7509,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -7396,7 +7526,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7413,7 +7543,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7430,7 +7560,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7447,7 +7577,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7464,7 +7594,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7481,7 +7611,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7498,7 +7628,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7515,7 +7645,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7532,7 +7662,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7549,7 +7679,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7566,7 +7696,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7583,7 +7713,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7600,7 +7730,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7617,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7634,7 +7764,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7651,7 +7781,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7668,7 +7798,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7685,7 +7815,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7702,7 +7832,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7719,7 +7849,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7749,16 +7879,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7775,7 +7905,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -7792,7 +7922,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -7809,7 +7939,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7826,7 +7956,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7843,7 +7973,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -7860,7 +7990,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
Relabels Total Revenue and Total Expenses to Operating Revenue and Operating Expenses. Edits the code/formulas/data to support this. Adds UAL Q4 and FY 2025 results except for long term debt. Adds UAL Q4 2025 insights. Remaining UAL FY result and insights awaiting release of 10-K.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{180469F5-A0EE-40E9-991D-66A7579DB96B}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9187A247-A46C-49C9-80EF-1678F1AA4EAB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Airline</t>
   </si>
   <si>
-    <t>Total Revenue</t>
-  </si>
-  <si>
     <t>Net Income</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
   </si>
   <si>
     <t>Passenger Revenue</t>
-  </si>
-  <si>
-    <t>Total Expenses</t>
   </si>
   <si>
     <t>RPM</t>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>Shares Sold</t>
+  </si>
+  <si>
+    <t>Operating Revenue</t>
+  </si>
+  <si>
+    <t>Operating Expenses</t>
   </si>
 </sst>
 </file>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G194" sqref="G194"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K198" sqref="K198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,9 +971,10 @@
     <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.109375" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -991,28 +992,28 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1023,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>10401000000</v>
@@ -1055,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>9968000000</v>
@@ -1087,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>9032000000</v>
@@ -1119,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>11643000000</v>
@@ -1151,7 +1152,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>11775000000</v>
@@ -1183,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>10777000000</v>
@@ -1215,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>11559000000</v>
@@ -1247,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>11953000000</v>
@@ -1279,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>11003000000</v>
@@ -1311,7 +1312,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>10938000000</v>
@@ -1343,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>10742000000</v>
@@ -1375,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>10491000000</v>
@@ -1404,10 +1405,10 @@
         <v>2018</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>44541000000</v>
@@ -1439,10 +1440,10 @@
         <v>2018</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>44438000000</v>
@@ -1474,10 +1475,10 @@
         <v>2018</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>41303000000</v>
@@ -1512,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>10584000000</v>
@@ -1544,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>10472000000</v>
@@ -1576,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>9589000000</v>
@@ -1608,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>11960000000</v>
@@ -1640,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>12536000000</v>
@@ -1672,7 +1673,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>11402000000</v>
@@ -1704,7 +1705,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>11911000000</v>
@@ -1736,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24">
         <v>12560000000</v>
@@ -1768,7 +1769,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>11380000000</v>
@@ -1800,7 +1801,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26">
         <v>11313000000</v>
@@ -1832,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27">
         <v>11439000000</v>
@@ -1864,7 +1865,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <v>10888000000</v>
@@ -1893,10 +1894,10 @@
         <v>2019</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29">
         <v>45768000000</v>
@@ -1928,10 +1929,10 @@
         <v>2019</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <v>47007000000</v>
@@ -1963,10 +1964,10 @@
         <v>2019</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>43259000000</v>
@@ -2001,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>8515000000</v>
@@ -2033,7 +2034,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33">
         <v>8592000000</v>
@@ -2065,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>7979000000</v>
@@ -2097,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35">
         <v>1622000000</v>
@@ -2129,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>1468000000</v>
@@ -2161,7 +2162,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <v>1475000000</v>
@@ -2193,7 +2194,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38">
         <v>3173000000</v>
@@ -2225,7 +2226,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>3062000000</v>
@@ -2257,7 +2258,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40">
         <v>2489000000</v>
@@ -2289,7 +2290,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>4027000000</v>
@@ -2321,7 +2322,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42">
         <v>3973000000</v>
@@ -2353,7 +2354,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43">
         <v>3412000000</v>
@@ -2382,10 +2383,10 @@
         <v>2020</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>17337000000</v>
@@ -2417,10 +2418,10 @@
         <v>2020</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D45">
         <v>17095000000</v>
@@ -2452,10 +2453,10 @@
         <v>2020</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46">
         <v>15355000000</v>
@@ -2490,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>4008000000</v>
@@ -2522,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D48">
         <v>4150000000</v>
@@ -2554,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49">
         <v>3221000000</v>
@@ -2586,7 +2587,7 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>7478000000</v>
@@ -2618,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51">
         <v>7126000000</v>
@@ -2650,7 +2651,7 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52">
         <v>5471000000</v>
@@ -2682,7 +2683,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D53">
         <v>8969000000</v>
@@ -2714,7 +2715,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54">
         <v>9154000000</v>
@@ -2746,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D55">
         <v>7750000000</v>
@@ -2778,7 +2779,7 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D56">
         <v>9427000000</v>
@@ -2810,7 +2811,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D57">
         <v>9470000000</v>
@@ -2842,7 +2843,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D58">
         <v>8192000000</v>
@@ -2871,10 +2872,10 @@
         <v>2021</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D59">
         <v>29882000000</v>
@@ -2906,10 +2907,10 @@
         <v>2021</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60">
         <v>29899000000</v>
@@ -2941,10 +2942,10 @@
         <v>2021</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61">
         <v>24634000000</v>
@@ -2979,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62">
         <v>8899000000</v>
@@ -3011,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D63">
         <v>9348000000</v>
@@ -3043,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D64">
         <v>7566000000</v>
@@ -3075,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65">
         <v>13422000000</v>
@@ -3107,7 +3108,7 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D66">
         <v>13824000000</v>
@@ -3139,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67">
         <v>12112000000</v>
@@ -3171,7 +3172,7 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D68">
         <v>13462000000</v>
@@ -3203,7 +3204,7 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D69">
         <v>13975000000</v>
@@ -3235,7 +3236,7 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D70">
         <v>12877000000</v>
@@ -3267,7 +3268,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D71">
         <v>13189000000</v>
@@ -3299,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D72">
         <v>13435000000</v>
@@ -3331,7 +3332,7 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D73">
         <v>12400000000</v>
@@ -3360,10 +3361,10 @@
         <v>2022</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74">
         <v>48971000000</v>
@@ -3395,10 +3396,10 @@
         <v>2022</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D75">
         <v>50582000000</v>
@@ -3430,10 +3431,10 @@
         <v>2022</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D76">
         <v>44955000000</v>
@@ -3468,7 +3469,7 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77">
         <v>12189000000</v>
@@ -3500,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D78">
         <v>12759000000</v>
@@ -3532,7 +3533,7 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D79">
         <v>11429000000</v>
@@ -3564,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D80">
         <v>14055000000</v>
@@ -3596,7 +3597,7 @@
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81">
         <v>15578000000</v>
@@ -3628,7 +3629,7 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D82">
         <v>14178000000</v>
@@ -3660,7 +3661,7 @@
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D83">
         <v>13482000000</v>
@@ -3692,7 +3693,7 @@
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D84">
         <v>15488000000</v>
@@ -3724,7 +3725,7 @@
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D85">
         <v>14484000000</v>
@@ -3756,7 +3757,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D86">
         <v>13062000000</v>
@@ -3788,7 +3789,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D87">
         <v>14223000000</v>
@@ -3820,7 +3821,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D88">
         <v>13626000000</v>
@@ -3849,10 +3850,10 @@
         <v>2023</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D89">
         <v>52788000000</v>
@@ -3884,10 +3885,10 @@
         <v>2023</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D90">
         <v>58048000000</v>
@@ -3919,10 +3920,10 @@
         <v>2023</v>
       </c>
       <c r="B91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91">
         <v>53717000000</v>
@@ -3957,7 +3958,7 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D92">
         <v>12570000000</v>
@@ -3990,7 +3991,7 @@
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D93">
         <v>13748000000</v>
@@ -4022,7 +4023,7 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D94">
         <v>12539000000</v>
@@ -4054,7 +4055,7 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D95">
         <v>14334000000</v>
@@ -4087,7 +4088,7 @@
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D96">
         <v>16658000000</v>
@@ -4119,7 +4120,7 @@
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97">
         <v>14986000000</v>
@@ -4151,7 +4152,7 @@
         <v>3</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D98">
         <v>13647000000</v>
@@ -4184,7 +4185,7 @@
         <v>3</v>
       </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D99">
         <v>15677000000</v>
@@ -4216,7 +4217,7 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D100">
         <v>14843000000</v>
@@ -4245,10 +4246,10 @@
         <v>2017</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D101">
         <v>42207000000</v>
@@ -4280,10 +4281,10 @@
         <v>2016</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D102">
         <v>40180000000</v>
@@ -4315,10 +4316,10 @@
         <v>2015</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D103">
         <v>40990000000</v>
@@ -4350,10 +4351,10 @@
         <v>2014</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D104">
         <v>42650000000</v>
@@ -4385,10 +4386,10 @@
         <v>2017</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D105">
         <v>41244000000</v>
@@ -4420,10 +4421,10 @@
         <v>2016</v>
       </c>
       <c r="B106" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D106">
         <v>39639000000</v>
@@ -4455,10 +4456,10 @@
         <v>2015</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D107">
         <v>40704000000</v>
@@ -4490,10 +4491,10 @@
         <v>2014</v>
       </c>
       <c r="B108" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D108">
         <v>40362000000</v>
@@ -4525,10 +4526,10 @@
         <v>2017</v>
       </c>
       <c r="B109" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D109">
         <v>37736000000</v>
@@ -4560,10 +4561,10 @@
         <v>2016</v>
       </c>
       <c r="B110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C110" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D110">
         <v>36556000000</v>
@@ -4595,10 +4596,10 @@
         <v>2015</v>
       </c>
       <c r="B111" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D111">
         <v>37864000000</v>
@@ -4630,10 +4631,10 @@
         <v>2014</v>
       </c>
       <c r="B112" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D112">
         <v>38901000000</v>
@@ -4665,10 +4666,10 @@
         <v>2023</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D113">
         <v>26091000000</v>
@@ -4700,10 +4701,10 @@
         <v>2022</v>
       </c>
       <c r="B114" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D114">
         <v>23814000000</v>
@@ -4735,10 +4736,10 @@
         <v>2021</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C115" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D115">
         <v>15790000000</v>
@@ -4770,10 +4771,10 @@
         <v>2020</v>
       </c>
       <c r="B116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D116">
         <v>9048000000</v>
@@ -4805,10 +4806,10 @@
         <v>2019</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D117">
         <v>22428000000</v>
@@ -4840,10 +4841,10 @@
         <v>2018</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D118">
         <v>21965000000</v>
@@ -4875,10 +4876,10 @@
         <v>2017</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D119">
         <v>21171000000</v>
@@ -4910,10 +4911,10 @@
         <v>2016</v>
       </c>
       <c r="B120" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D120">
         <v>20425000000</v>
@@ -4945,10 +4946,10 @@
         <v>2015</v>
       </c>
       <c r="B121" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D121">
         <v>19820000000</v>
@@ -4980,10 +4981,10 @@
         <v>2014</v>
       </c>
       <c r="B122" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D122">
         <v>18605000000</v>
@@ -5018,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D123">
         <v>6870000000</v>
@@ -5050,7 +5051,7 @@
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D124">
         <v>7354000000</v>
@@ -5082,7 +5083,7 @@
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D125">
         <v>6329000000</v>
@@ -5114,7 +5115,7 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D126">
         <v>9624000000</v>
@@ -5146,7 +5147,7 @@
         <v>2</v>
       </c>
       <c r="C127" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D127">
         <v>11105000000</v>
@@ -5178,7 +5179,7 @@
         <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D128">
         <v>10878000000</v>
@@ -5210,7 +5211,7 @@
         <v>4</v>
       </c>
       <c r="C129" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D129">
         <v>10600000000</v>
@@ -5242,7 +5243,7 @@
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D130">
         <v>9435000000</v>
@@ -5274,7 +5275,7 @@
         <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D131">
         <v>10363000000</v>
@@ -5306,7 +5307,7 @@
         <v>3</v>
       </c>
       <c r="C132" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D132">
         <v>10594000000</v>
@@ -5338,7 +5339,7 @@
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D133">
         <v>9789000000</v>
@@ -5370,7 +5371,7 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D134">
         <v>9827000000</v>
@@ -5402,7 +5403,7 @@
         <v>2</v>
       </c>
       <c r="C135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D135">
         <v>10827000000</v>
@@ -5434,7 +5435,7 @@
         <v>3</v>
       </c>
       <c r="C136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D136">
         <v>10706000000</v>
@@ -5466,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D137">
         <v>9630000000</v>
@@ -5498,7 +5499,7 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D138">
         <v>9995000000</v>
@@ -5530,7 +5531,7 @@
         <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D139">
         <v>11355000000</v>
@@ -5562,7 +5563,7 @@
         <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D140">
         <v>11139000000</v>
@@ -5594,7 +5595,7 @@
         <v>4</v>
       </c>
       <c r="C141" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D141">
         <v>10160000000</v>
@@ -5626,7 +5627,7 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D142">
         <v>9148000000</v>
@@ -5658,7 +5659,7 @@
         <v>2</v>
       </c>
       <c r="C143" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D143">
         <v>10791000000</v>
@@ -5690,7 +5691,7 @@
         <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D144">
         <v>11060000000</v>
@@ -5722,7 +5723,7 @@
         <v>4</v>
       </c>
       <c r="C145" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D145">
         <v>10245000000</v>
@@ -5754,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D146">
         <v>9251000000</v>
@@ -5786,7 +5787,7 @@
         <v>2</v>
       </c>
       <c r="C147" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D147">
         <v>10447000000</v>
@@ -5818,7 +5819,7 @@
         <v>3</v>
       </c>
       <c r="C148" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D148">
         <v>10483000000</v>
@@ -5850,7 +5851,7 @@
         <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D149">
         <v>9458000000</v>
@@ -5882,7 +5883,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D150">
         <v>9388000000</v>
@@ -5914,7 +5915,7 @@
         <v>2</v>
       </c>
       <c r="C151" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D151">
         <v>10707000000</v>
@@ -5946,7 +5947,7 @@
         <v>3</v>
       </c>
       <c r="C152" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D152">
         <v>11107000000</v>
@@ -5978,7 +5979,7 @@
         <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D153">
         <v>9502000000</v>
@@ -6010,7 +6011,7 @@
         <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D154">
         <v>8916000000</v>
@@ -6042,7 +6043,7 @@
         <v>2</v>
       </c>
       <c r="C155" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D155">
         <v>10621000000</v>
@@ -6074,7 +6075,7 @@
         <v>3</v>
       </c>
       <c r="C156" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D156">
         <v>11178000000</v>
@@ -6106,7 +6107,7 @@
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D157">
         <v>9647000000</v>
@@ -6138,7 +6139,7 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D158">
         <v>8420000000</v>
@@ -6170,7 +6171,7 @@
         <v>2</v>
       </c>
       <c r="C159" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D159">
         <v>10000000000</v>
@@ -6202,7 +6203,7 @@
         <v>3</v>
       </c>
       <c r="C160" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D160">
         <v>9878000000</v>
@@ -6234,7 +6235,7 @@
         <v>4</v>
       </c>
       <c r="C161" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D161">
         <v>9438000000</v>
@@ -6266,7 +6267,7 @@
         <v>1</v>
       </c>
       <c r="C162" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D162">
         <v>8195000000</v>
@@ -6298,7 +6299,7 @@
         <v>2</v>
       </c>
       <c r="C163" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D163">
         <v>9396000000</v>
@@ -6330,7 +6331,7 @@
         <v>3</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D164">
         <v>9913000000</v>
@@ -6362,7 +6363,7 @@
         <v>4</v>
       </c>
       <c r="C165" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D165">
         <v>9052000000</v>
@@ -6394,7 +6395,7 @@
         <v>1</v>
       </c>
       <c r="C166" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D166">
         <v>8608000000</v>
@@ -6426,7 +6427,7 @@
         <v>2</v>
       </c>
       <c r="C167" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D167">
         <v>9914000000</v>
@@ -6458,7 +6459,7 @@
         <v>3</v>
       </c>
       <c r="C168" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D168">
         <v>10306000000</v>
@@ -6490,7 +6491,7 @@
         <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D169">
         <v>9036000000</v>
@@ -6522,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="C170" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D170">
         <v>8696000000</v>
@@ -6554,7 +6555,7 @@
         <v>2</v>
       </c>
       <c r="C171" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D171">
         <v>10329000000</v>
@@ -6586,7 +6587,7 @@
         <v>3</v>
       </c>
       <c r="C172" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D172">
         <v>10563000000</v>
@@ -6618,7 +6619,7 @@
         <v>4</v>
       </c>
       <c r="C173" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D173">
         <v>9313000000</v>
@@ -6650,7 +6651,7 @@
         <v>4</v>
       </c>
       <c r="C174" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D174">
         <v>15559000000</v>
@@ -6679,10 +6680,10 @@
         <v>2024</v>
       </c>
       <c r="B175" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D175">
         <v>61643000000</v>
@@ -6717,7 +6718,7 @@
         <v>4</v>
       </c>
       <c r="C176" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D176">
         <v>14695000000</v>
@@ -6746,10 +6747,10 @@
         <v>2024</v>
       </c>
       <c r="B177" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D177">
         <v>57063000000</v>
@@ -6784,7 +6785,7 @@
         <v>4</v>
       </c>
       <c r="C178" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D178">
         <v>13660000000</v>
@@ -6814,10 +6815,10 @@
         <v>2024</v>
       </c>
       <c r="B179" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D179">
         <v>54211000000</v>
@@ -6852,7 +6853,7 @@
         <v>4</v>
       </c>
       <c r="C180" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D180">
         <v>6931000000</v>
@@ -6881,10 +6882,10 @@
         <v>2024</v>
       </c>
       <c r="B181" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C181" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D181">
         <v>27483000000</v>
@@ -6919,7 +6920,7 @@
         <v>1</v>
       </c>
       <c r="C182" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D182">
         <v>14040000000</v>
@@ -6951,7 +6952,7 @@
         <v>1</v>
       </c>
       <c r="C183" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D183">
         <v>13213000000</v>
@@ -6983,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="C184" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D184">
         <v>12551000000</v>
@@ -7015,7 +7016,7 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D185">
         <v>6428000000</v>
@@ -7047,7 +7048,7 @@
         <v>2</v>
       </c>
       <c r="C186" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D186">
         <v>16648000000</v>
@@ -7079,7 +7080,7 @@
         <v>2</v>
       </c>
       <c r="C187" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D187">
         <v>15236000000</v>
@@ -7111,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="C188" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D188">
         <v>14392000000</v>
@@ -7140,7 +7141,7 @@
         <v>2</v>
       </c>
       <c r="C189" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D189">
         <v>7244000000</v>
@@ -7172,7 +7173,7 @@
         <v>3</v>
       </c>
       <c r="C190" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D190">
         <v>16673000000</v>
@@ -7204,7 +7205,7 @@
         <v>3</v>
       </c>
       <c r="C191" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D191">
         <v>15225000000</v>
@@ -7236,7 +7237,7 @@
         <v>3</v>
       </c>
       <c r="C192" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D192">
         <v>13691000000</v>
@@ -7268,7 +7269,7 @@
         <v>3</v>
       </c>
       <c r="C193" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D193">
         <v>6949000000</v>
@@ -7300,7 +7301,7 @@
         <v>4</v>
       </c>
       <c r="C194" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D194">
         <v>16003000000</v>
@@ -7329,10 +7330,10 @@
         <v>2025</v>
       </c>
       <c r="B195" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D195">
         <v>63364000000</v>
@@ -7364,7 +7365,28 @@
         <v>4</v>
       </c>
       <c r="C196" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D196">
+        <v>15397000000</v>
+      </c>
+      <c r="E196">
+        <v>13926000000</v>
+      </c>
+      <c r="F196">
+        <v>14011000000</v>
+      </c>
+      <c r="G196">
+        <v>1044000000</v>
+      </c>
+      <c r="H196">
+        <v>68246000000</v>
+      </c>
+      <c r="I196">
+        <v>83365000000</v>
+      </c>
+      <c r="K196">
+        <v>244000000</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.3">
@@ -7372,10 +7394,31 @@
         <v>2025</v>
       </c>
       <c r="B197" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D197">
+        <v>59070000000</v>
+      </c>
+      <c r="E197">
+        <v>53438000000</v>
+      </c>
+      <c r="F197">
+        <v>54356000000</v>
+      </c>
+      <c r="G197">
+        <v>3353000000</v>
+      </c>
+      <c r="H197">
+        <v>271619000000</v>
+      </c>
+      <c r="I197">
+        <v>330284000000</v>
+      </c>
+      <c r="K197">
+        <v>704000000</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.3">
@@ -7386,7 +7429,7 @@
         <v>4</v>
       </c>
       <c r="C198" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.3">
@@ -7394,10 +7437,10 @@
         <v>2025</v>
       </c>
       <c r="B199" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C199" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.3">
@@ -7408,7 +7451,7 @@
         <v>4</v>
       </c>
       <c r="C200" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.3">
@@ -7416,10 +7459,10 @@
         <v>2025</v>
       </c>
       <c r="B201" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C201" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7452,10 +7495,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -7463,10 +7506,10 @@
         <v>2013</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7480,10 +7523,10 @@
         <v>2014</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>23400000</v>
@@ -7497,10 +7540,10 @@
         <v>2015</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>85100000</v>
@@ -7514,10 +7557,10 @@
         <v>2016</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>119800000</v>
@@ -7531,10 +7574,10 @@
         <v>2017</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>33900000</v>
@@ -7548,10 +7591,10 @@
         <v>2018</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>16600000</v>
@@ -7565,10 +7608,10 @@
         <v>2019</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>33800000</v>
@@ -7582,10 +7625,10 @@
         <v>2020</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>6400000</v>
@@ -7599,10 +7642,10 @@
         <v>2013</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>10000000</v>
@@ -7616,10 +7659,10 @@
         <v>2014</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>28600000</v>
@@ -7633,10 +7676,10 @@
         <v>2015</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>48400000</v>
@@ -7650,10 +7693,10 @@
         <v>2016</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>60000000</v>
@@ -7667,10 +7710,10 @@
         <v>2017</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>33000000</v>
@@ -7684,10 +7727,10 @@
         <v>2018</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>29000000</v>
@@ -7701,10 +7744,10 @@
         <v>2019</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>38000000</v>
@@ -7718,10 +7761,10 @@
         <v>2020</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>6700000</v>
@@ -7735,10 +7778,10 @@
         <v>2013</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -7752,10 +7795,10 @@
         <v>2014</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>6500000</v>
@@ -7769,10 +7812,10 @@
         <v>2015</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>21000000</v>
@@ -7786,10 +7829,10 @@
         <v>2016</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>50000000</v>
@@ -7803,10 +7846,10 @@
         <v>2017</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>28000000</v>
@@ -7820,10 +7863,10 @@
         <v>2018</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>17500000</v>
@@ -7837,10 +7880,10 @@
         <v>2019</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <v>19200000</v>
@@ -7854,10 +7897,10 @@
         <v>2020</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>4300000</v>
@@ -7899,10 +7942,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -7910,10 +7953,10 @@
         <v>2020</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>143597509</v>
@@ -7927,10 +7970,10 @@
         <v>2021</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>79599019</v>
@@ -7944,10 +7987,10 @@
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>6500000</v>
@@ -7961,10 +8004,10 @@
         <v>2021</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>2100000</v>
@@ -7978,10 +8021,10 @@
         <v>2020</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>69338841</v>
@@ -7995,10 +8038,10 @@
         <v>2021</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>14200000</v>

</xml_diff>

<commit_message>
Adds AAL Q4 and FY 2025 results except for long term debt and profit sharing. Adds AAL Q4 2025 insights. Remaining AAL results and FY insights awaiting release of 10-K.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9187A247-A46C-49C9-80EF-1678F1AA4EAB}"/>
+  <xr:revisionPtr revIDLastSave="426" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67404081-827D-44F5-98B0-CC21B910CEA6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -962,26 +962,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K198" sqref="K198"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K179" sqref="K179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>610559</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>120716144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>7762816</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6067,7 +6067,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>98910482</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2025</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>124000000</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2025</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2025</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>2025</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>2025</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>470000000</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2025</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>2025</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>77636000000</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>2025</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>2025</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>392000000</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>2025</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>2025</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>2025</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>2025</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>351000000</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>2025</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>1337000000</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>2025</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>244000000</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>2025</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>704000000</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>2025</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2025</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2025</v>
       </c>
@@ -7453,8 +7453,26 @@
       <c r="C200" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D200">
+        <v>13999000000</v>
+      </c>
+      <c r="E200">
+        <v>12657000000</v>
+      </c>
+      <c r="F200">
+        <v>13548000000</v>
+      </c>
+      <c r="G200">
+        <v>99000000</v>
+      </c>
+      <c r="H200">
+        <v>61596000000</v>
+      </c>
+      <c r="I200">
+        <v>74472000000</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>2025</v>
       </c>
@@ -7463,6 +7481,24 @@
       </c>
       <c r="C201" t="s">
         <v>5</v>
+      </c>
+      <c r="D201">
+        <v>54633000000</v>
+      </c>
+      <c r="E201">
+        <v>49643000000</v>
+      </c>
+      <c r="F201">
+        <v>53166000000</v>
+      </c>
+      <c r="G201">
+        <v>111000000</v>
+      </c>
+      <c r="H201">
+        <v>250294000000</v>
+      </c>
+      <c r="I201">
+        <v>299411000000</v>
       </c>
     </row>
   </sheetData>
@@ -7478,13 +7514,13 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7501,7 +7537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -7518,7 +7554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -7535,7 +7571,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -7552,7 +7588,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -7569,7 +7605,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7586,7 +7622,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7603,7 +7639,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7620,7 +7656,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7637,7 +7673,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7654,7 +7690,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7671,7 +7707,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7688,7 +7724,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7705,7 +7741,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7722,7 +7758,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7739,7 +7775,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7756,7 +7792,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7773,7 +7809,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7790,7 +7826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7807,7 +7843,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7824,7 +7860,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7841,7 +7877,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7858,7 +7894,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7875,7 +7911,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7892,7 +7928,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7922,16 +7958,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7948,7 +7984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -7965,7 +8001,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -7982,7 +8018,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7999,7 +8035,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -8016,7 +8052,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -8033,7 +8069,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
Adds LUV Q4 and FY 2025 results except for long term debt. Adds LUV Q4 2025 insights. Remaining DAL FY result and insights awaiting release of 10-K.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67404081-827D-44F5-98B0-CC21B910CEA6}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB32AECD-AEE1-478A-B96E-366C2C5FE689}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -962,26 +962,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K179" sqref="K179"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I199" sqref="I199"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>610559</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>120716144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>7762816</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6067,7 +6067,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>98910482</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>2025</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>124000000</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2025</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>2025</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2025</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2025</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>470000000</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2025</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2025</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>77636000000</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2025</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2025</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>392000000</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2025</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2025</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2025</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2025</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>351000000</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2025</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>1337000000</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>2025</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>244000000</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>2025</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>704000000</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2025</v>
       </c>
@@ -7431,8 +7431,29 @@
       <c r="C198" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D198">
+        <v>7442000000</v>
+      </c>
+      <c r="E198">
+        <v>6785000000</v>
+      </c>
+      <c r="F198">
+        <v>7051000000</v>
+      </c>
+      <c r="G198">
+        <v>323000000</v>
+      </c>
+      <c r="H198">
+        <v>35567000000</v>
+      </c>
+      <c r="I198">
+        <v>46052000000</v>
+      </c>
+      <c r="K198">
+        <v>71000000</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>2025</v>
       </c>
@@ -7442,8 +7463,29 @@
       <c r="C199" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D199">
+        <v>28063000000</v>
+      </c>
+      <c r="E199">
+        <v>25535000000</v>
+      </c>
+      <c r="F199">
+        <v>27635000000</v>
+      </c>
+      <c r="G199">
+        <v>441000000</v>
+      </c>
+      <c r="H199">
+        <v>139443000000</v>
+      </c>
+      <c r="I199">
+        <v>180046000000</v>
+      </c>
+      <c r="K199">
+        <v>97000000</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>2025</v>
       </c>
@@ -7472,7 +7514,7 @@
         <v>74472000000</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>2025</v>
       </c>
@@ -7514,13 +7556,13 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7537,7 +7579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -7554,7 +7596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -7571,7 +7613,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -7588,7 +7630,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -7605,7 +7647,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7622,7 +7664,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7639,7 +7681,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7656,7 +7698,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7673,7 +7715,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7690,7 +7732,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7707,7 +7749,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7724,7 +7766,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7741,7 +7783,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7758,7 +7800,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7775,7 +7817,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7792,7 +7834,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7809,7 +7851,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7826,7 +7868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7843,7 +7885,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7860,7 +7902,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7877,7 +7919,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7894,7 +7936,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7911,7 +7953,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7928,7 +7970,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -7958,16 +8000,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7984,7 +8026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -8001,7 +8043,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -8018,7 +8060,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -8035,7 +8077,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -8052,7 +8094,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -8069,7 +8111,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
Adds remaining metrics and FY insights for 2025 from 10-K annual filings for all airlines. Adds callout of resumption of share repurchases if applicable.
</commit_message>
<xml_diff>
--- a/airline_financial_data.xlsx
+++ b/airline_financial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f26b992e1a44723/Documents/School/UNCC/Personal Projects/US Airlines Financials Project/airline_financials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="441" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB32AECD-AEE1-478A-B96E-366C2C5FE689}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="8_{5FE741C9-A2F0-4D0A-8E2F-B83D587BBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E3FC9C9-A1B5-4890-BE0E-70BB459607B8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5CC2E0DD-0C2A-471D-BE08-E27D8B31800B}"/>
   </bookViews>
   <sheets>
     <sheet name="airline_financials" sheetId="2" r:id="rId1"/>
@@ -639,10 +639,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -962,26 +958,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF35CD-6CF2-4D2E-9294-3A1A732D8FBE}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I199" sqref="I199"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K206" sqref="K206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1048,7 +1044,7 @@
         <v>29000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -1080,7 +1076,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1112,7 +1108,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1144,7 +1140,7 @@
         <v>63000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1176,7 +1172,7 @@
         <v>404000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1208,7 +1204,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -1240,7 +1236,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -1272,7 +1268,7 @@
         <v>399000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1304,7 +1300,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1336,7 +1332,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -1368,7 +1364,7 @@
         <v>311000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -1400,7 +1396,7 @@
         <v>82000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -1435,7 +1431,7 @@
         <v>175000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1470,7 +1466,7 @@
         <v>1301000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1505,7 +1501,7 @@
         <v>334000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1537,7 +1533,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -1569,7 +1565,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -1601,7 +1597,7 @@
         <v>33000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1633,7 +1629,7 @@
         <v>67000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -1665,7 +1661,7 @@
         <v>518000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1697,7 +1693,7 @@
         <v>161000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -1729,7 +1725,7 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -1761,7 +1757,7 @@
         <v>517000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -1793,7 +1789,7 @@
         <v>174000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1825,7 +1821,7 @@
         <v>74000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1857,7 +1853,7 @@
         <v>387000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1889,7 +1885,7 @@
         <v>123000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1924,7 +1920,7 @@
         <v>213000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1959,7 +1955,7 @@
         <v>1643000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1994,7 +1990,7 @@
         <v>491000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -2026,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -2058,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2090,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2122,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2154,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2186,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2218,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2250,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2020</v>
       </c>
@@ -2282,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2314,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -2346,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2020</v>
       </c>
@@ -2378,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2020</v>
       </c>
@@ -2413,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -2448,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2020</v>
       </c>
@@ -2483,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2515,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2547,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2579,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2611,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2643,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2675,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2707,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2739,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2771,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2803,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2835,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2867,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2902,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2937,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2972,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -3004,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -3036,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -3068,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -3100,7 +3096,7 @@
         <v>64000000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -3132,7 +3128,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -3164,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -3196,7 +3192,7 @@
         <v>59000000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -3228,7 +3224,7 @@
         <v>237000000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3260,7 +3256,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -3292,7 +3288,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -3324,7 +3320,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -3356,7 +3352,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3391,7 +3387,7 @@
         <v>211000000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -3426,7 +3422,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -3461,7 +3457,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2023</v>
       </c>
@@ -3493,7 +3489,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2023</v>
       </c>
@@ -3525,7 +3521,7 @@
         <v>72000000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2023</v>
       </c>
@@ -3557,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -3589,7 +3585,7 @@
         <v>173000000</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2023</v>
       </c>
@@ -3621,7 +3617,7 @@
         <v>595000000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2023</v>
       </c>
@@ -3653,7 +3649,7 @@
         <v>220000000</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -3685,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -3717,7 +3713,7 @@
         <v>417000000</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2023</v>
       </c>
@@ -3749,7 +3745,7 @@
         <v>301000000</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2023</v>
       </c>
@@ -3781,7 +3777,7 @@
         <v>53000000</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -3813,7 +3809,7 @@
         <v>299000000</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2023</v>
       </c>
@@ -3845,7 +3841,7 @@
         <v>160000000</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2023</v>
       </c>
@@ -3880,7 +3876,7 @@
         <v>261000000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2023</v>
       </c>
@@ -3915,7 +3911,7 @@
         <v>1383000000</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -3950,7 +3946,7 @@
         <v>681000000</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -3983,7 +3979,7 @@
         <v>610559</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -4015,7 +4011,7 @@
         <v>125000000</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -4047,7 +4043,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -4080,7 +4076,7 @@
         <v>120716144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -4112,7 +4108,7 @@
         <v>519000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -4144,7 +4140,7 @@
         <v>185000000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -4177,7 +4173,7 @@
         <v>7762816</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -4209,7 +4205,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4241,7 +4237,7 @@
         <v>231000000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2017</v>
       </c>
@@ -4276,7 +4272,7 @@
         <v>241000000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4311,7 +4307,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2015</v>
       </c>
@@ -4346,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -4381,7 +4377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2017</v>
       </c>
@@ -4416,7 +4412,7 @@
         <v>1065000000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4451,7 +4447,7 @@
         <v>1115000000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2015</v>
       </c>
@@ -4486,7 +4482,7 @@
         <v>1490000000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -4521,7 +4517,7 @@
         <v>1085000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4556,7 +4552,7 @@
         <v>349000000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2016</v>
       </c>
@@ -4591,7 +4587,7 @@
         <v>628000000</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4626,7 +4622,7 @@
         <v>698000000</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -4661,7 +4657,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -4696,7 +4692,7 @@
         <v>110000000</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2022</v>
       </c>
@@ -4731,7 +4727,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -4766,7 +4762,7 @@
         <v>230000000</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -4801,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4836,7 +4832,7 @@
         <v>695000000</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -4871,7 +4867,7 @@
         <v>580000000</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -4906,7 +4902,7 @@
         <v>579000000</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2016</v>
       </c>
@@ -4941,7 +4937,7 @@
         <v>645000000</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -4976,7 +4972,7 @@
         <v>655000000</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2014</v>
       </c>
@@ -5011,7 +5007,7 @@
         <v>374000000</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -5043,7 +5039,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -5075,7 +5071,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -5107,7 +5103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2017</v>
       </c>
@@ -5139,7 +5135,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2017</v>
       </c>
@@ -5171,7 +5167,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2017</v>
       </c>
@@ -5203,7 +5199,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2017</v>
       </c>
@@ -5235,7 +5231,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -5267,7 +5263,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -5299,7 +5295,7 @@
         <v>98000000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -5331,7 +5327,7 @@
         <v>86000000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -5363,7 +5359,7 @@
         <v>57000000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2015</v>
       </c>
@@ -5395,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2015</v>
       </c>
@@ -5427,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2015</v>
       </c>
@@ -5459,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2015</v>
       </c>
@@ -5491,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -5523,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -5555,7 +5551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -5587,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -5619,7 +5615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2017</v>
       </c>
@@ -5651,7 +5647,7 @@
         <v>151000000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2017</v>
       </c>
@@ -5683,7 +5679,7 @@
         <v>338000000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2017</v>
       </c>
@@ -5715,7 +5711,7 @@
         <v>314000000</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2017</v>
       </c>
@@ -5747,7 +5743,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2016</v>
       </c>
@@ -5779,7 +5775,7 @@
         <v>272000000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2016</v>
       </c>
@@ -5811,7 +5807,7 @@
         <v>324000000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2016</v>
       </c>
@@ -5843,7 +5839,7 @@
         <v>326000000</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2016</v>
       </c>
@@ -5875,7 +5871,7 @@
         <v>193000000</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -5907,7 +5903,7 @@
         <v>136000000</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2015</v>
       </c>
@@ -5939,7 +5935,7 @@
         <v>411000000</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2015</v>
       </c>
@@ -5971,7 +5967,7 @@
         <v>563000000</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2015</v>
       </c>
@@ -6003,7 +5999,7 @@
         <v>380000000</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -6035,7 +6031,7 @@
         <v>99000000</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -6067,7 +6063,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -6099,7 +6095,7 @@
         <v>384000000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -6131,7 +6127,7 @@
         <v>262000000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -6163,7 +6159,7 @@
         <v>28000000</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -6195,7 +6191,7 @@
         <v>140000000</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -6227,7 +6223,7 @@
         <v>109000000</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -6259,7 +6255,7 @@
         <v>73000000</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2016</v>
       </c>
@@ -6291,7 +6287,7 @@
         <v>94000000</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2016</v>
       </c>
@@ -6323,7 +6319,7 @@
         <v>153000000</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2016</v>
       </c>
@@ -6355,7 +6351,7 @@
         <v>235000000</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2016</v>
       </c>
@@ -6387,7 +6383,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2015</v>
       </c>
@@ -6419,7 +6415,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2015</v>
       </c>
@@ -6451,7 +6447,7 @@
         <v>195000000</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2015</v>
       </c>
@@ -6483,7 +6479,7 @@
         <v>257000000</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2015</v>
       </c>
@@ -6515,7 +6511,7 @@
         <v>146000000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2014</v>
       </c>
@@ -6547,7 +6543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2014</v>
       </c>
@@ -6579,7 +6575,7 @@
         <v>78000000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2014</v>
       </c>
@@ -6611,7 +6607,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2014</v>
       </c>
@@ -6643,7 +6639,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -6675,7 +6671,7 @@
         <v>425000000</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -6710,7 +6706,7 @@
         <v>1389000000</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -6742,7 +6738,7 @@
         <v>294000000</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -6777,7 +6773,7 @@
         <v>713000000</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2024</v>
       </c>
@@ -6810,7 +6806,7 @@
         <v>98910482</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2024</v>
       </c>
@@ -6845,7 +6841,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -6877,7 +6873,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2024</v>
       </c>
@@ -6912,7 +6908,7 @@
         <v>103000000</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2025</v>
       </c>
@@ -6944,7 +6940,7 @@
         <v>124000000</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2025</v>
       </c>
@@ -6976,7 +6972,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2025</v>
       </c>
@@ -7008,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>2025</v>
       </c>
@@ -7040,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>2025</v>
       </c>
@@ -7072,7 +7068,7 @@
         <v>470000000</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2025</v>
       </c>
@@ -7104,7 +7100,7 @@
         <v>188000000</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>2025</v>
       </c>
@@ -7132,8 +7128,12 @@
       <c r="I188">
         <v>77636000000</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K188">
+        <f>ROUND($K$201*(((D188-F188)/($D$201-$F$201))/(((D200-F200)/($D$201-$F$201))+((D188-F188)/($D$201-$F$201)))),0)</f>
+        <v>39360025</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>2025</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>2025</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>392000000</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>2025</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>228000000</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>2025</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>2025</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>2025</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>351000000</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>2025</v>
       </c>
@@ -7353,11 +7353,14 @@
       <c r="I195">
         <v>298045000000</v>
       </c>
+      <c r="J195">
+        <v>11936000000</v>
+      </c>
       <c r="K195">
         <v>1337000000</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>2025</v>
       </c>
@@ -7389,7 +7392,7 @@
         <v>244000000</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>2025</v>
       </c>
@@ -7417,11 +7420,14 @@
       <c r="I197">
         <v>330284000000</v>
       </c>
+      <c r="J197">
+        <v>17170000000</v>
+      </c>
       <c r="K197">
         <v>704000000</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>2025</v>
       </c>
@@ -7453,7 +7459,7 @@
         <v>71000000</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2025</v>
       </c>
@@ -7481,11 +7487,14 @@
       <c r="I199">
         <v>180046000000</v>
       </c>
+      <c r="J199">
+        <v>4577000000</v>
+      </c>
       <c r="K199">
         <v>97000000</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2025</v>
       </c>
@@ -7513,8 +7522,12 @@
       <c r="I200">
         <v>74472000000</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K200">
+        <f>ROUND($K$201*(((D200-F200)/($D$201-$F$201))/(((D200-F200)/($D$201-$F$201))+((D188-F188)/($D$201-$F$201)))),0)</f>
+        <v>15639975</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>2025</v>
       </c>
@@ -7541,6 +7554,12 @@
       </c>
       <c r="I201">
         <v>299411000000</v>
+      </c>
+      <c r="J201">
+        <v>24639000000</v>
+      </c>
+      <c r="K201">
+        <v>55000000</v>
       </c>
     </row>
   </sheetData>
@@ -7556,13 +7575,13 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7579,7 +7598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -7596,7 +7615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -7613,7 +7632,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -7630,7 +7649,7 @@
         <v>3600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -7647,7 +7666,7 @@
         <v>4400000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -7664,7 +7683,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7681,7 +7700,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7698,7 +7717,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -7715,7 +7734,7 @@
         <v>145000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -7732,7 +7751,7 @@
         <v>250000000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -7749,7 +7768,7 @@
         <v>1100000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -7766,7 +7785,7 @@
         <v>2200000000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7783,7 +7802,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -7800,7 +7819,7 @@
         <v>1700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -7817,7 +7836,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -7834,7 +7853,7 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -7851,7 +7870,7 @@
         <v>377620000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -7868,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -7885,7 +7904,7 @@
         <v>320000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -7902,7 +7921,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -7919,7 +7938,7 @@
         <v>2600000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -7936,7 +7955,7 @@
         <v>1800000000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -7953,7 +7972,7 @@
         <v>1200000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -7970,7 +7989,7 @@
         <v>1600000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -8000,16 +8019,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8026,7 +8045,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -8043,7 +8062,7 @@
         <v>1901355562.5899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -8060,7 +8079,7 @@
         <v>1082205377.28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -8077,7 +8096,7 @@
         <v>158535000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -8094,7 +8113,7 @@
         <v>83433000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -8111,7 +8130,7 @@
         <v>2293578491.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2021</v>
       </c>

</xml_diff>